<commit_message>
Update of some files
</commit_message>
<xml_diff>
--- a/private/INDIVIDUAL_LOCALIZATIONS_UI_1.xlsx
+++ b/private/INDIVIDUAL_LOCALIZATIONS_UI_1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\WebApps\lol\private\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\LolVvv\Assets\private\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="687">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="778">
   <si>
     <t>en_US</t>
   </si>
@@ -2088,6 +2088,279 @@
   </si>
   <si>
     <t>pt_BR</t>
+  </si>
+  <si>
+    <t>apart</t>
+  </si>
+  <si>
+    <t>Apart</t>
+  </si>
+  <si>
+    <t>Einzeln</t>
+  </si>
+  <si>
+    <t>free</t>
+  </si>
+  <si>
+    <t>Free</t>
+  </si>
+  <si>
+    <t>Frei</t>
+  </si>
+  <si>
+    <t>starterItems</t>
+  </si>
+  <si>
+    <t>Starter Items</t>
+  </si>
+  <si>
+    <t>Startgegenstände</t>
+  </si>
+  <si>
+    <t>mostPopularSetup</t>
+  </si>
+  <si>
+    <t>mostPopularItems</t>
+  </si>
+  <si>
+    <t>Most Popular Setup</t>
+  </si>
+  <si>
+    <t>Most Popular Items</t>
+  </si>
+  <si>
+    <t>Meistgenutztes Setup</t>
+  </si>
+  <si>
+    <t>Meistgenutzte Gegenstände</t>
+  </si>
+  <si>
+    <t>finalTrinket</t>
+  </si>
+  <si>
+    <t>Final Trinket</t>
+  </si>
+  <si>
+    <t>Finales Totem</t>
+  </si>
+  <si>
+    <t>finalBoots</t>
+  </si>
+  <si>
+    <t>Final Boots</t>
+  </si>
+  <si>
+    <t>Finale Schuhe</t>
+  </si>
+  <si>
+    <t>O nas</t>
+  </si>
+  <si>
+    <t>Ostatnie mecze</t>
+  </si>
+  <si>
+    <t>Ostatnie wyszukiwania</t>
+  </si>
+  <si>
+    <t>Ulubieni</t>
+  </si>
+  <si>
+    <t>Bohaterowie</t>
+  </si>
+  <si>
+    <t>Profesjonaliści</t>
+  </si>
+  <si>
+    <t>Pokaż więcej …</t>
+  </si>
+  <si>
+    <t>Ładowanie …</t>
+  </si>
+  <si>
+    <t>Szukanie …</t>
+  </si>
+  <si>
+    <t>Szukaj bohaterów i profesjonalistów</t>
+  </si>
+  <si>
+    <t>Szukaj bohatera</t>
+  </si>
+  <si>
+    <t>Szukaj profesjonalisty</t>
+  </si>
+  <si>
+    <t>Nie znaleziono pasujących meczu!</t>
+  </si>
+  <si>
+    <t>Nie znaleziono pasujących bohaterów!</t>
+  </si>
+  <si>
+    <t>Nie znaleziono pasujących profesjonalistów!</t>
+  </si>
+  <si>
+    <t>Nie znaleziono bohatera w podanym URL!</t>
+  </si>
+  <si>
+    <t>Nie znaleziono profesjonalisty w podanym URL!</t>
+  </si>
+  <si>
+    <t>Nie znaeziono meczu w podanym URL!</t>
+  </si>
+  <si>
+    <t>Skontaktuj się z nami w razie błędu.</t>
+  </si>
+  <si>
+    <t>Wiadomość wysłana pomyślnie</t>
+  </si>
+  <si>
+    <t>Otrzymaliśmy Twoją wiadomość i postaramy się odpowiedzieć w jak najszybszym tempie. Dziękujemy za skontaktowanie się z nami.</t>
+  </si>
+  <si>
+    <t>Imię</t>
+  </si>
+  <si>
+    <t>Temat</t>
+  </si>
+  <si>
+    <t>Wiadomość</t>
+  </si>
+  <si>
+    <t>Zostaw nam wiadomość …</t>
+  </si>
+  <si>
+    <t>Wyślij</t>
+  </si>
+  <si>
+    <t>Wystąpił błąd</t>
+  </si>
+  <si>
+    <t>Prosimy rozwiąż CAPTCHA przed wysłaniem zgłoszenia.</t>
+  </si>
+  <si>
+    <t>Spróbuj użyć innych kryteriów</t>
+  </si>
+  <si>
+    <t>maks</t>
+  </si>
+  <si>
+    <t>Długość meczu</t>
+  </si>
+  <si>
+    <t>Wiek {wiek}</t>
+  </si>
+  <si>
+    <t>Przełamania</t>
+  </si>
+  <si>
+    <t>Analiza</t>
+  </si>
+  <si>
+    <t>Wynik</t>
+  </si>
+  <si>
+    <t>Przeciwnik</t>
+  </si>
+  <si>
+    <t>Rozegrano</t>
+  </si>
+  <si>
+    <t>Podsumowanie</t>
+  </si>
+  <si>
+    <t>Uczestnicy</t>
+  </si>
+  <si>
+    <t>Statystyki</t>
+  </si>
+  <si>
+    <t>Najbardziej popularne</t>
+  </si>
+  <si>
+    <t>Według kupionych przedmiotów</t>
+  </si>
+  <si>
+    <t>Według rozdanych umiejętności</t>
+  </si>
+  <si>
+    <t>Ukończony build</t>
+  </si>
+  <si>
+    <t>Runa kluczowa</t>
+  </si>
+  <si>
+    <t>Runa większa</t>
+  </si>
+  <si>
+    <t>Pozycja</t>
+  </si>
+  <si>
+    <t>Idealne</t>
+  </si>
+  <si>
+    <t>Udział w zabójstwach</t>
+  </si>
+  <si>
+    <t>Góra</t>
+  </si>
+  <si>
+    <t>Dżungla</t>
+  </si>
+  <si>
+    <t>Środek</t>
+  </si>
+  <si>
+    <t>Strzelec</t>
+  </si>
+  <si>
+    <t>Wsparcie</t>
+  </si>
+  <si>
+    <t>Ranga</t>
+  </si>
+  <si>
+    <t>Osobno</t>
+  </si>
+  <si>
+    <t>Darmowa</t>
+  </si>
+  <si>
+    <t>Wygrana</t>
+  </si>
+  <si>
+    <t>W grze</t>
+  </si>
+  <si>
+    <t>Zwycięstwo</t>
+  </si>
+  <si>
+    <t>Porażka</t>
+  </si>
+  <si>
+    <t>Najbardziej popularny układ</t>
+  </si>
+  <si>
+    <t>Najbardziej popularne przedmioty</t>
+  </si>
+  <si>
+    <t>Początkowe przedmioty</t>
+  </si>
+  <si>
+    <t>Końcowy trinket</t>
+  </si>
+  <si>
+    <t>Końcowe buty</t>
+  </si>
+  <si>
+    <t>Skontaktuj się z nami</t>
+  </si>
+  <si>
+    <t>Ujawnenie prawne</t>
+  </si>
+  <si>
+    <t>Polityka prywatności</t>
+  </si>
+  <si>
+    <t>Pierwsza zniszczona wieża</t>
   </si>
 </sst>
 </file>
@@ -2550,13 +2823,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U104"/>
+  <dimension ref="A1:U111"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="J5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="L60" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K8" sqref="K8"/>
+      <selection pane="bottomRight" activeCell="N71" sqref="N71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2655,6 +2928,9 @@
       <c r="C2" s="4" t="s">
         <v>598</v>
       </c>
+      <c r="N2" s="4" t="s">
+        <v>708</v>
+      </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -2666,6 +2942,9 @@
       <c r="C3" s="4" t="s">
         <v>597</v>
       </c>
+      <c r="N3" s="4" t="s">
+        <v>597</v>
+      </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -2677,6 +2956,9 @@
       <c r="C4" s="4" t="s">
         <v>87</v>
       </c>
+      <c r="N4" s="4" t="s">
+        <v>709</v>
+      </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -2688,6 +2970,9 @@
       <c r="C5" s="4" t="s">
         <v>122</v>
       </c>
+      <c r="N5" s="4" t="s">
+        <v>710</v>
+      </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
@@ -2699,6 +2984,9 @@
       <c r="C6" s="4" t="s">
         <v>125</v>
       </c>
+      <c r="N6" s="4" t="s">
+        <v>711</v>
+      </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -2710,6 +2998,9 @@
       <c r="C7" s="4" t="s">
         <v>287</v>
       </c>
+      <c r="N7" s="4" t="s">
+        <v>712</v>
+      </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -2721,6 +3012,9 @@
       <c r="C8" s="4" t="s">
         <v>289</v>
       </c>
+      <c r="N8" s="4" t="s">
+        <v>713</v>
+      </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
@@ -2732,6 +3026,9 @@
       <c r="C9" s="4" t="s">
         <v>69</v>
       </c>
+      <c r="N9" s="4" t="s">
+        <v>714</v>
+      </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
@@ -2743,6 +3040,9 @@
       <c r="C10" s="4" t="s">
         <v>334</v>
       </c>
+      <c r="N10" s="4" t="s">
+        <v>715</v>
+      </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -2754,6 +3054,9 @@
       <c r="C11" s="4" t="s">
         <v>107</v>
       </c>
+      <c r="N11" s="4" t="s">
+        <v>716</v>
+      </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
@@ -2765,6 +3068,9 @@
       <c r="C12" s="4" t="s">
         <v>292</v>
       </c>
+      <c r="N12" s="4" t="s">
+        <v>717</v>
+      </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
@@ -2776,6 +3082,9 @@
       <c r="C13" s="4" t="s">
         <v>112</v>
       </c>
+      <c r="N13" s="4" t="s">
+        <v>718</v>
+      </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
@@ -2787,6 +3096,9 @@
       <c r="C14" s="4" t="s">
         <v>113</v>
       </c>
+      <c r="N14" s="4" t="s">
+        <v>719</v>
+      </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
@@ -2798,6 +3110,9 @@
       <c r="C15" s="4" t="s">
         <v>85</v>
       </c>
+      <c r="N15" s="4" t="s">
+        <v>720</v>
+      </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
@@ -2809,8 +3124,11 @@
       <c r="C16" s="4" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="N16" s="4" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>116</v>
       </c>
@@ -2820,8 +3138,11 @@
       <c r="C17" s="4" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="N17" s="4" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>293</v>
       </c>
@@ -2831,8 +3152,11 @@
       <c r="C18" s="4" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="N18" s="4" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>294</v>
       </c>
@@ -2842,8 +3166,11 @@
       <c r="C19" s="4" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="N19" s="4" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>320</v>
       </c>
@@ -2853,8 +3180,11 @@
       <c r="C20" s="4" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="N20" s="4" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>298</v>
       </c>
@@ -2864,8 +3194,11 @@
       <c r="C21" s="4" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="N21" s="4" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>622</v>
       </c>
@@ -2875,8 +3208,11 @@
       <c r="C22" s="9" t="s">
         <v>621</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="N22" s="4" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>623</v>
       </c>
@@ -2886,8 +3222,11 @@
       <c r="C23" s="9" t="s">
         <v>625</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="N23" s="4" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>626</v>
       </c>
@@ -2897,8 +3236,11 @@
       <c r="C24" s="9" t="s">
         <v>640</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="N24" s="4" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>627</v>
       </c>
@@ -2908,8 +3250,11 @@
       <c r="C25" s="9" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="N25" s="4" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>629</v>
       </c>
@@ -2919,8 +3264,11 @@
       <c r="C26" s="9" t="s">
         <v>637</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="N26" s="4" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>630</v>
       </c>
@@ -2930,8 +3278,11 @@
       <c r="C27" s="9" t="s">
         <v>636</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="N27" s="4" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>631</v>
       </c>
@@ -2941,8 +3292,11 @@
       <c r="C28" s="9" t="s">
         <v>642</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="N28" s="4" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>632</v>
       </c>
@@ -2952,8 +3306,11 @@
       <c r="C29" s="9" t="s">
         <v>634</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="N29" s="4" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>643</v>
       </c>
@@ -2963,8 +3320,11 @@
       <c r="C30" s="9" t="s">
         <v>647</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="N30" s="4" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>645</v>
       </c>
@@ -2974,8 +3334,11 @@
       <c r="C31" s="9" t="s">
         <v>648</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="N31" s="4" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>72</v>
       </c>
@@ -2985,8 +3348,11 @@
       <c r="C32" s="4" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="N32" s="4" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>74</v>
       </c>
@@ -2996,8 +3362,11 @@
       <c r="C33" s="4" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="N33" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>77</v>
       </c>
@@ -3007,8 +3376,11 @@
       <c r="C34" s="4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="N34" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>78</v>
       </c>
@@ -3018,8 +3390,11 @@
       <c r="C35" s="4" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="N35" s="4" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>82</v>
       </c>
@@ -3029,8 +3404,11 @@
       <c r="C36" s="4" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="N36" s="4" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>249</v>
       </c>
@@ -3040,8 +3418,11 @@
       <c r="C37" s="4" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="N37" s="4" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>252</v>
       </c>
@@ -3051,8 +3432,11 @@
       <c r="C38" s="4" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="N38" s="4" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>254</v>
       </c>
@@ -3062,8 +3446,11 @@
       <c r="C39" s="4" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="N39" s="4" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>256</v>
       </c>
@@ -3073,8 +3460,11 @@
       <c r="C40" s="4" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="N40" s="4" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>257</v>
       </c>
@@ -3084,8 +3474,11 @@
       <c r="C41" s="4" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="N41" s="4" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>258</v>
       </c>
@@ -3095,8 +3488,11 @@
       <c r="C42" s="4" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="N42" s="4" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>310</v>
       </c>
@@ -3106,8 +3502,11 @@
       <c r="C43" s="4" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="N43" s="4" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>311</v>
       </c>
@@ -3117,8 +3516,11 @@
       <c r="C44" s="4" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="N44" s="4" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>312</v>
       </c>
@@ -3128,8 +3530,11 @@
       <c r="C45" s="4" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="N45" s="4" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>265</v>
       </c>
@@ -3139,8 +3544,11 @@
       <c r="C46" s="4" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="N46" s="4" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>649</v>
       </c>
@@ -3150,8 +3558,11 @@
       <c r="C47" s="9" t="s">
         <v>651</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="N47" s="4" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>263</v>
       </c>
@@ -3161,8 +3572,11 @@
       <c r="C48" s="4" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N48" s="4" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>283</v>
       </c>
@@ -3172,8 +3586,11 @@
       <c r="C49" s="4" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N49" s="4" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>276</v>
       </c>
@@ -3183,8 +3600,11 @@
       <c r="C50" s="4" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N50" s="4" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>279</v>
       </c>
@@ -3194,8 +3614,11 @@
       <c r="C51" s="4" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N51" s="4" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>683</v>
       </c>
@@ -3205,8 +3628,11 @@
       <c r="C52" s="9" t="s">
         <v>684</v>
       </c>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N52" s="4" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>281</v>
       </c>
@@ -3216,8 +3642,11 @@
       <c r="C53" s="4" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N53" s="4" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>302</v>
       </c>
@@ -3227,8 +3656,11 @@
       <c r="C54" s="4" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N54" s="4" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>304</v>
       </c>
@@ -3238,8 +3670,11 @@
       <c r="C55" s="4" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N55" s="4" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>307</v>
       </c>
@@ -3249,48 +3684,66 @@
       <c r="C56" s="4" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N56" s="4" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>323</v>
       </c>
       <c r="B57" s="4" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N57" s="4" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>327</v>
       </c>
       <c r="B58" s="4" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N58" s="4" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>324</v>
       </c>
       <c r="B59" s="4" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N59" s="4" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>325</v>
       </c>
       <c r="B60" s="4" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N60" s="4" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>326</v>
       </c>
       <c r="B61" s="4" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N61" s="4" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>336</v>
       </c>
@@ -3300,1719 +3753,1854 @@
       <c r="C62" s="4" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N62" s="4" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>339</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>340</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>341</v>
-      </c>
-      <c r="J63" s="5"/>
-      <c r="K63" s="5"/>
-      <c r="O63" s="5"/>
-    </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+        <v>687</v>
+      </c>
+      <c r="B63" s="9" t="s">
+        <v>688</v>
+      </c>
+      <c r="C63" s="9" t="s">
+        <v>689</v>
+      </c>
+      <c r="N63" s="4" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>612</v>
-      </c>
-      <c r="B64" s="4" t="s">
-        <v>613</v>
-      </c>
-      <c r="C64" s="4" t="s">
-        <v>614</v>
-      </c>
-      <c r="J64" s="5"/>
-      <c r="K64" s="5"/>
-      <c r="O64" s="5"/>
+        <v>690</v>
+      </c>
+      <c r="B64" s="9" t="s">
+        <v>691</v>
+      </c>
+      <c r="C64" s="9" t="s">
+        <v>692</v>
+      </c>
+      <c r="N64" s="4" t="s">
+        <v>764</v>
+      </c>
     </row>
     <row r="65" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>606</v>
+        <v>339</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>609</v>
-      </c>
-      <c r="C65" s="9" t="s">
-        <v>609</v>
+        <v>340</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>341</v>
       </c>
       <c r="J65" s="5"/>
       <c r="K65" s="5"/>
+      <c r="N65" s="4" t="s">
+        <v>765</v>
+      </c>
       <c r="O65" s="5"/>
     </row>
     <row r="66" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>607</v>
+        <v>612</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>610</v>
-      </c>
-      <c r="C66" s="9" t="s">
-        <v>615</v>
+        <v>613</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>614</v>
       </c>
       <c r="J66" s="5"/>
       <c r="K66" s="5"/>
+      <c r="N66" s="4" t="s">
+        <v>766</v>
+      </c>
       <c r="O66" s="5"/>
     </row>
     <row r="67" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>616</v>
+        <v>609</v>
       </c>
       <c r="J67" s="5"/>
       <c r="K67" s="5"/>
+      <c r="N67" s="4" t="s">
+        <v>609</v>
+      </c>
       <c r="O67" s="5"/>
     </row>
     <row r="68" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>617</v>
-      </c>
-      <c r="B68" s="9" t="s">
-        <v>618</v>
+        <v>607</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>610</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
       <c r="J68" s="5"/>
       <c r="K68" s="5"/>
+      <c r="N68" s="4" t="s">
+        <v>767</v>
+      </c>
       <c r="O68" s="5"/>
     </row>
     <row r="69" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>600</v>
+        <v>608</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>603</v>
-      </c>
-      <c r="C69" s="4" t="s">
-        <v>604</v>
+        <v>611</v>
+      </c>
+      <c r="C69" s="9" t="s">
+        <v>616</v>
       </c>
       <c r="J69" s="5"/>
       <c r="K69" s="5"/>
+      <c r="N69" s="4" t="s">
+        <v>768</v>
+      </c>
       <c r="O69" s="5"/>
     </row>
     <row r="70" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
+        <v>696</v>
+      </c>
+      <c r="B70" s="9" t="s">
+        <v>698</v>
+      </c>
+      <c r="C70" s="9" t="s">
+        <v>700</v>
+      </c>
+      <c r="J70" s="5"/>
+      <c r="K70" s="5"/>
+      <c r="N70" s="4" t="s">
+        <v>769</v>
+      </c>
+      <c r="O70" s="5"/>
+    </row>
+    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A71" s="3" t="s">
+        <v>697</v>
+      </c>
+      <c r="B71" s="9" t="s">
+        <v>699</v>
+      </c>
+      <c r="C71" s="9" t="s">
+        <v>701</v>
+      </c>
+      <c r="J71" s="5"/>
+      <c r="K71" s="5"/>
+      <c r="N71" s="4" t="s">
+        <v>770</v>
+      </c>
+      <c r="O71" s="5"/>
+    </row>
+    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A72" s="3" t="s">
+        <v>693</v>
+      </c>
+      <c r="B72" s="9" t="s">
+        <v>694</v>
+      </c>
+      <c r="C72" s="9" t="s">
+        <v>695</v>
+      </c>
+      <c r="J72" s="5"/>
+      <c r="K72" s="5"/>
+      <c r="N72" s="4" t="s">
+        <v>771</v>
+      </c>
+      <c r="O72" s="5"/>
+    </row>
+    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A73" s="3" t="s">
+        <v>702</v>
+      </c>
+      <c r="B73" s="9" t="s">
+        <v>703</v>
+      </c>
+      <c r="C73" s="9" t="s">
+        <v>704</v>
+      </c>
+      <c r="J73" s="5"/>
+      <c r="K73" s="5"/>
+      <c r="N73" s="4" t="s">
+        <v>772</v>
+      </c>
+      <c r="O73" s="5"/>
+    </row>
+    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A74" s="3" t="s">
+        <v>705</v>
+      </c>
+      <c r="B74" s="9" t="s">
+        <v>706</v>
+      </c>
+      <c r="C74" s="9" t="s">
+        <v>707</v>
+      </c>
+      <c r="J74" s="5"/>
+      <c r="K74" s="5"/>
+      <c r="N74" s="4" t="s">
+        <v>773</v>
+      </c>
+      <c r="O74" s="5"/>
+    </row>
+    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A75" s="3" t="s">
+        <v>617</v>
+      </c>
+      <c r="B75" s="9" t="s">
+        <v>618</v>
+      </c>
+      <c r="C75" s="9" t="s">
+        <v>619</v>
+      </c>
+      <c r="J75" s="5"/>
+      <c r="K75" s="5"/>
+      <c r="N75" s="4" t="s">
+        <v>774</v>
+      </c>
+      <c r="O75" s="5"/>
+    </row>
+    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A76" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>603</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>604</v>
+      </c>
+      <c r="J76" s="5"/>
+      <c r="K76" s="5"/>
+      <c r="N76" s="4" t="s">
+        <v>775</v>
+      </c>
+      <c r="O76" s="5"/>
+    </row>
+    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A77" s="3" t="s">
         <v>601</v>
       </c>
-      <c r="B70" s="4" t="s">
+      <c r="B77" s="4" t="s">
         <v>602</v>
       </c>
-      <c r="C70" s="4" t="s">
+      <c r="C77" s="4" t="s">
         <v>605</v>
       </c>
-      <c r="K70" s="10"/>
-      <c r="L70" s="10"/>
-      <c r="M70" s="10"/>
-      <c r="N70" s="10"/>
-      <c r="O70" s="5"/>
-    </row>
-    <row r="71" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B71" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C71" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="D71" s="8" t="s">
-        <v>501</v>
-      </c>
-      <c r="E71" s="8" t="s">
-        <v>470</v>
-      </c>
-      <c r="F71" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="G71" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="H71" s="8" t="s">
-        <v>407</v>
-      </c>
-      <c r="K71" s="10" t="s">
-        <v>562</v>
-      </c>
-      <c r="L71" s="10" t="s">
-        <v>652</v>
-      </c>
-      <c r="M71" s="10"/>
-      <c r="N71" s="10" t="s">
-        <v>439</v>
-      </c>
-      <c r="O71" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="P71" s="8" t="s">
-        <v>375</v>
-      </c>
-      <c r="Q71" s="8" t="s">
-        <v>217</v>
-      </c>
-      <c r="S71" s="7" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="72" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B72" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C72" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D72" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E72" s="8" t="s">
-        <v>471</v>
-      </c>
-      <c r="F72" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="G72" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="H72" s="8" t="s">
-        <v>408</v>
-      </c>
-      <c r="K72" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="L72" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="M72" s="10"/>
-      <c r="N72" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="O72" s="8" t="s">
-        <v>531</v>
-      </c>
-      <c r="P72" s="8" t="s">
-        <v>376</v>
-      </c>
-      <c r="Q72" s="8" t="s">
-        <v>218</v>
-      </c>
-      <c r="S72" s="7" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="73" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B73" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C73" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="D73" s="8" t="s">
-        <v>502</v>
-      </c>
-      <c r="E73" s="8" t="s">
-        <v>472</v>
-      </c>
-      <c r="F73" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="G73" s="8" t="s">
-        <v>187</v>
-      </c>
-      <c r="H73" s="8" t="s">
-        <v>409</v>
-      </c>
-      <c r="K73" s="10" t="s">
-        <v>563</v>
-      </c>
-      <c r="L73" s="10" t="s">
-        <v>653</v>
-      </c>
-      <c r="M73" s="10"/>
-      <c r="N73" s="10" t="s">
-        <v>440</v>
-      </c>
-      <c r="O73" s="8" t="s">
-        <v>532</v>
-      </c>
-      <c r="P73" s="8" t="s">
-        <v>377</v>
-      </c>
-      <c r="Q73" s="8" t="s">
-        <v>219</v>
-      </c>
-      <c r="S73" s="7" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="74" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B74" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C74" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="D74" s="8" t="s">
-        <v>503</v>
-      </c>
-      <c r="E74" s="8" t="s">
-        <v>473</v>
-      </c>
-      <c r="F74" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="G74" s="8" t="s">
-        <v>188</v>
-      </c>
-      <c r="H74" s="8" t="s">
-        <v>410</v>
-      </c>
-      <c r="K74" s="10" t="s">
-        <v>564</v>
-      </c>
-      <c r="L74" s="10" t="s">
-        <v>654</v>
-      </c>
-      <c r="M74" s="10"/>
-      <c r="N74" s="10" t="s">
-        <v>441</v>
-      </c>
-      <c r="O74" s="8" t="s">
-        <v>533</v>
-      </c>
-      <c r="P74" s="8" t="s">
-        <v>378</v>
-      </c>
-      <c r="Q74" s="8" t="s">
-        <v>220</v>
-      </c>
-      <c r="S74" s="7" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="75" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B75" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C75" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="D75" s="8" t="s">
-        <v>504</v>
-      </c>
-      <c r="E75" s="8" t="s">
-        <v>474</v>
-      </c>
-      <c r="F75" s="8" t="s">
-        <v>159</v>
-      </c>
-      <c r="G75" s="8" t="s">
-        <v>189</v>
-      </c>
-      <c r="H75" s="8" t="s">
-        <v>411</v>
-      </c>
-      <c r="K75" s="10" t="s">
-        <v>565</v>
-      </c>
-      <c r="L75" s="10" t="s">
-        <v>655</v>
-      </c>
-      <c r="M75" s="10"/>
-      <c r="N75" s="10" t="s">
-        <v>442</v>
-      </c>
-      <c r="O75" s="8" t="s">
-        <v>534</v>
-      </c>
-      <c r="P75" s="8" t="s">
-        <v>379</v>
-      </c>
-      <c r="Q75" s="8" t="s">
-        <v>221</v>
-      </c>
-      <c r="S75" s="7" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="76" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="B76" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="C76" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="D76" s="8" t="s">
-        <v>505</v>
-      </c>
-      <c r="E76" s="8" t="s">
-        <v>475</v>
-      </c>
-      <c r="F76" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="G76" s="8" t="s">
-        <v>190</v>
-      </c>
-      <c r="H76" s="8" t="s">
-        <v>412</v>
-      </c>
-      <c r="K76" s="10" t="s">
-        <v>566</v>
-      </c>
-      <c r="L76" s="10" t="s">
-        <v>656</v>
-      </c>
-      <c r="M76" s="10"/>
-      <c r="N76" s="10" t="s">
-        <v>443</v>
-      </c>
-      <c r="O76" s="8" t="s">
-        <v>535</v>
-      </c>
-      <c r="P76" s="8" t="s">
-        <v>380</v>
-      </c>
-      <c r="Q76" s="8" t="s">
-        <v>222</v>
-      </c>
-      <c r="S76" s="7" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="77" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B77" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C77" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="D77" s="8" t="s">
-        <v>506</v>
-      </c>
-      <c r="E77" s="8" t="s">
-        <v>476</v>
-      </c>
-      <c r="F77" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="G77" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="H77" s="8" t="s">
-        <v>413</v>
-      </c>
-      <c r="K77" s="10" t="s">
-        <v>567</v>
-      </c>
-      <c r="L77" s="10" t="s">
-        <v>657</v>
-      </c>
-      <c r="M77" s="10"/>
-      <c r="N77" s="10" t="s">
-        <v>444</v>
-      </c>
-      <c r="O77" s="8" t="s">
-        <v>536</v>
-      </c>
-      <c r="P77" s="8" t="s">
-        <v>381</v>
-      </c>
-      <c r="Q77" s="8" t="s">
-        <v>223</v>
-      </c>
-      <c r="S77" s="7" t="s">
-        <v>349</v>
-      </c>
+      <c r="N77" s="4" t="s">
+        <v>776</v>
+      </c>
+      <c r="O77" s="5"/>
     </row>
     <row r="78" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="6" t="s">
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="C78" s="8" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="D78" s="8" t="s">
-        <v>507</v>
+        <v>501</v>
       </c>
       <c r="E78" s="8" t="s">
-        <v>477</v>
+        <v>470</v>
       </c>
       <c r="F78" s="8" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="G78" s="8" t="s">
-        <v>192</v>
+        <v>60</v>
       </c>
       <c r="H78" s="8" t="s">
-        <v>414</v>
+        <v>407</v>
       </c>
       <c r="K78" s="10" t="s">
-        <v>568</v>
+        <v>562</v>
       </c>
       <c r="L78" s="10" t="s">
-        <v>658</v>
+        <v>652</v>
       </c>
       <c r="M78" s="10"/>
       <c r="N78" s="10" t="s">
-        <v>445</v>
+        <v>439</v>
       </c>
       <c r="O78" s="8" t="s">
-        <v>537</v>
+        <v>155</v>
       </c>
       <c r="P78" s="8" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="Q78" s="8" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="S78" s="7" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
     </row>
     <row r="79" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="C79" s="8" t="s">
-        <v>133</v>
+        <v>7</v>
       </c>
       <c r="D79" s="8" t="s">
-        <v>508</v>
+        <v>7</v>
       </c>
       <c r="E79" s="8" t="s">
-        <v>478</v>
+        <v>471</v>
       </c>
       <c r="F79" s="8" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="G79" s="8" t="s">
-        <v>193</v>
+        <v>7</v>
       </c>
       <c r="H79" s="8" t="s">
-        <v>415</v>
+        <v>408</v>
       </c>
       <c r="K79" s="10" t="s">
-        <v>569</v>
+        <v>7</v>
       </c>
       <c r="L79" s="10" t="s">
-        <v>659</v>
+        <v>7</v>
       </c>
       <c r="M79" s="10"/>
       <c r="N79" s="10" t="s">
-        <v>446</v>
+        <v>7</v>
       </c>
       <c r="O79" s="8" t="s">
-        <v>538</v>
+        <v>531</v>
       </c>
       <c r="P79" s="8" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="Q79" s="8" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="S79" s="7" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
     </row>
     <row r="80" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="6" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C80" s="8" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="D80" s="8" t="s">
-        <v>509</v>
+        <v>502</v>
       </c>
       <c r="E80" s="8" t="s">
-        <v>479</v>
+        <v>472</v>
       </c>
       <c r="F80" s="8" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="G80" s="8" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="H80" s="8" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
       <c r="K80" s="10" t="s">
-        <v>570</v>
+        <v>563</v>
       </c>
       <c r="L80" s="10" t="s">
-        <v>660</v>
+        <v>653</v>
       </c>
       <c r="M80" s="10"/>
       <c r="N80" s="10" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
       <c r="O80" s="8" t="s">
-        <v>539</v>
+        <v>532</v>
       </c>
       <c r="P80" s="8" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="Q80" s="8" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="S80" s="7" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
     </row>
     <row r="81" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="6" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C81" s="8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D81" s="8" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="E81" s="8" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="F81" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G81" s="8" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H81" s="8" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="K81" s="10" t="s">
-        <v>571</v>
+        <v>564</v>
       </c>
       <c r="L81" s="10" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="M81" s="10"/>
       <c r="N81" s="10" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="O81" s="8" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="P81" s="8" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="Q81" s="8" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="S81" s="7" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="82" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="6" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C82" s="8" t="s">
-        <v>271</v>
+        <v>129</v>
       </c>
       <c r="D82" s="8" t="s">
-        <v>510</v>
+        <v>504</v>
       </c>
       <c r="E82" s="8" t="s">
-        <v>480</v>
+        <v>474</v>
       </c>
       <c r="F82" s="8" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="G82" s="8" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="H82" s="8" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
       <c r="K82" s="10" t="s">
-        <v>572</v>
+        <v>565</v>
       </c>
       <c r="L82" s="10" t="s">
-        <v>661</v>
+        <v>655</v>
       </c>
       <c r="M82" s="10"/>
       <c r="N82" s="10" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="O82" s="8" t="s">
-        <v>540</v>
+        <v>534</v>
       </c>
       <c r="P82" s="8" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
       <c r="Q82" s="8" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="S82" s="7" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
     </row>
     <row r="83" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="6" t="s">
-        <v>14</v>
+        <v>62</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="C83" s="8" t="s">
-        <v>270</v>
+        <v>130</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>511</v>
+        <v>505</v>
       </c>
       <c r="E83" s="8" t="s">
-        <v>481</v>
+        <v>475</v>
       </c>
       <c r="F83" s="8" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="G83" s="8" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="H83" s="8" t="s">
-        <v>418</v>
+        <v>412</v>
       </c>
       <c r="K83" s="10" t="s">
-        <v>573</v>
+        <v>566</v>
       </c>
       <c r="L83" s="10" t="s">
-        <v>662</v>
+        <v>656</v>
       </c>
       <c r="M83" s="10"/>
       <c r="N83" s="10" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="O83" s="8" t="s">
-        <v>541</v>
+        <v>535</v>
       </c>
       <c r="P83" s="8" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="Q83" s="8" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="S83" s="7" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
     </row>
     <row r="84" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="6" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="C84" s="8" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D84" s="8" t="s">
-        <v>512</v>
+        <v>506</v>
       </c>
       <c r="E84" s="8" t="s">
-        <v>482</v>
+        <v>476</v>
       </c>
       <c r="F84" s="8" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="G84" s="8" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="H84" s="8" t="s">
-        <v>419</v>
+        <v>413</v>
       </c>
       <c r="K84" s="10" t="s">
-        <v>574</v>
+        <v>567</v>
       </c>
       <c r="L84" s="10" t="s">
-        <v>663</v>
+        <v>657</v>
       </c>
       <c r="M84" s="10"/>
       <c r="N84" s="10" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="O84" s="8" t="s">
-        <v>542</v>
+        <v>536</v>
       </c>
       <c r="P84" s="8" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="Q84" s="8" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="S84" s="7" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
     </row>
     <row r="85" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="6" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C85" s="8" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D85" s="8" t="s">
-        <v>513</v>
+        <v>507</v>
       </c>
       <c r="E85" s="8" t="s">
-        <v>483</v>
+        <v>477</v>
       </c>
       <c r="F85" s="8" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="G85" s="8" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="H85" s="8" t="s">
-        <v>420</v>
+        <v>414</v>
       </c>
       <c r="K85" s="10" t="s">
-        <v>575</v>
+        <v>568</v>
       </c>
       <c r="L85" s="10" t="s">
-        <v>664</v>
+        <v>658</v>
       </c>
       <c r="M85" s="10"/>
       <c r="N85" s="10" t="s">
-        <v>451</v>
+        <v>445</v>
       </c>
       <c r="O85" s="8" t="s">
-        <v>543</v>
+        <v>537</v>
       </c>
       <c r="P85" s="8" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="Q85" s="8" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="S85" s="7" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
     </row>
     <row r="86" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="6" t="s">
-        <v>64</v>
+        <v>10</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="C86" s="8" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D86" s="8" t="s">
-        <v>514</v>
+        <v>508</v>
       </c>
       <c r="E86" s="8" t="s">
-        <v>484</v>
+        <v>478</v>
       </c>
       <c r="F86" s="8" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="G86" s="8" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="H86" s="8" t="s">
-        <v>421</v>
+        <v>415</v>
       </c>
       <c r="K86" s="10" t="s">
-        <v>576</v>
+        <v>569</v>
       </c>
       <c r="L86" s="10" t="s">
-        <v>665</v>
+        <v>659</v>
       </c>
       <c r="M86" s="10"/>
       <c r="N86" s="10" t="s">
-        <v>452</v>
+        <v>446</v>
       </c>
       <c r="O86" s="8" t="s">
-        <v>544</v>
+        <v>538</v>
       </c>
       <c r="P86" s="8" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
       <c r="Q86" s="8" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="S86" s="7" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
     </row>
     <row r="87" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="6" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C87" s="8" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D87" s="8" t="s">
-        <v>515</v>
+        <v>509</v>
       </c>
       <c r="E87" s="8" t="s">
-        <v>485</v>
+        <v>479</v>
       </c>
       <c r="F87" s="8" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="G87" s="8" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="H87" s="8" t="s">
-        <v>422</v>
+        <v>416</v>
       </c>
       <c r="K87" s="10" t="s">
-        <v>577</v>
+        <v>570</v>
       </c>
       <c r="L87" s="10" t="s">
-        <v>666</v>
+        <v>660</v>
       </c>
       <c r="M87" s="10"/>
       <c r="N87" s="10" t="s">
-        <v>453</v>
+        <v>447</v>
       </c>
       <c r="O87" s="8" t="s">
-        <v>545</v>
+        <v>539</v>
       </c>
       <c r="P87" s="8" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="Q87" s="8" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="S87" s="7" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
     </row>
     <row r="88" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="6" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C88" s="8" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="D88" s="8" t="s">
-        <v>516</v>
+        <v>505</v>
       </c>
       <c r="E88" s="8" t="s">
-        <v>486</v>
+        <v>475</v>
       </c>
       <c r="F88" s="8" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="G88" s="8" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="H88" s="8" t="s">
-        <v>423</v>
+        <v>412</v>
       </c>
       <c r="K88" s="10" t="s">
-        <v>578</v>
+        <v>571</v>
       </c>
       <c r="L88" s="10" t="s">
-        <v>667</v>
+        <v>656</v>
       </c>
       <c r="M88" s="10"/>
       <c r="N88" s="10" t="s">
-        <v>454</v>
+        <v>443</v>
       </c>
       <c r="O88" s="8" t="s">
-        <v>546</v>
+        <v>535</v>
       </c>
       <c r="P88" s="8" t="s">
-        <v>391</v>
+        <v>380</v>
       </c>
       <c r="Q88" s="8" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
       <c r="S88" s="7" t="s">
-        <v>359</v>
+        <v>348</v>
       </c>
     </row>
     <row r="89" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="6" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C89" s="8" t="s">
-        <v>140</v>
+        <v>271</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>517</v>
+        <v>510</v>
       </c>
       <c r="E89" s="8" t="s">
-        <v>487</v>
+        <v>480</v>
       </c>
       <c r="F89" s="8" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="G89" s="8" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="H89" s="8" t="s">
-        <v>424</v>
+        <v>417</v>
       </c>
       <c r="K89" s="10" t="s">
-        <v>579</v>
+        <v>572</v>
       </c>
       <c r="L89" s="10" t="s">
-        <v>668</v>
+        <v>661</v>
       </c>
       <c r="M89" s="10"/>
       <c r="N89" s="10" t="s">
-        <v>455</v>
+        <v>448</v>
       </c>
       <c r="O89" s="8" t="s">
-        <v>547</v>
+        <v>540</v>
       </c>
       <c r="P89" s="8" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
       <c r="Q89" s="8" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="S89" s="7" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
     </row>
     <row r="90" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="6" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C90" s="8" t="s">
-        <v>141</v>
+        <v>270</v>
       </c>
       <c r="D90" s="8" t="s">
-        <v>518</v>
+        <v>511</v>
       </c>
       <c r="E90" s="8" t="s">
-        <v>488</v>
+        <v>481</v>
       </c>
       <c r="F90" s="8" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="G90" s="8" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="H90" s="8" t="s">
-        <v>425</v>
+        <v>418</v>
       </c>
       <c r="K90" s="10" t="s">
-        <v>580</v>
+        <v>573</v>
       </c>
       <c r="L90" s="10" t="s">
-        <v>669</v>
+        <v>662</v>
       </c>
       <c r="M90" s="10"/>
       <c r="N90" s="10" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
       <c r="O90" s="8" t="s">
-        <v>548</v>
+        <v>541</v>
       </c>
       <c r="P90" s="8" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="Q90" s="8" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="S90" s="7" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
     </row>
     <row r="91" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C91" s="8" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="D91" s="8" t="s">
-        <v>519</v>
+        <v>512</v>
       </c>
       <c r="E91" s="8" t="s">
-        <v>489</v>
+        <v>482</v>
       </c>
       <c r="F91" s="8" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="G91" s="8" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="H91" s="8" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
       <c r="K91" s="10" t="s">
-        <v>581</v>
+        <v>574</v>
       </c>
       <c r="L91" s="10" t="s">
-        <v>670</v>
+        <v>663</v>
       </c>
       <c r="M91" s="10"/>
       <c r="N91" s="10" t="s">
-        <v>457</v>
+        <v>450</v>
       </c>
       <c r="O91" s="8" t="s">
-        <v>549</v>
+        <v>542</v>
       </c>
       <c r="P91" s="8" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
       <c r="Q91" s="8" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="S91" s="7" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
     </row>
     <row r="92" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="6" t="s">
-        <v>65</v>
+        <v>16</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>275</v>
+        <v>39</v>
       </c>
       <c r="C92" s="8" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="D92" s="8" t="s">
-        <v>458</v>
+        <v>513</v>
       </c>
       <c r="E92" s="8" t="s">
-        <v>490</v>
+        <v>483</v>
       </c>
       <c r="F92" s="8" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="G92" s="8" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="H92" s="8" t="s">
-        <v>427</v>
+        <v>420</v>
       </c>
       <c r="K92" s="10" t="s">
-        <v>582</v>
+        <v>575</v>
       </c>
       <c r="L92" s="10" t="s">
-        <v>671</v>
+        <v>664</v>
       </c>
       <c r="M92" s="10"/>
       <c r="N92" s="10" t="s">
-        <v>458</v>
+        <v>451</v>
       </c>
       <c r="O92" s="8" t="s">
-        <v>550</v>
+        <v>543</v>
       </c>
       <c r="P92" s="8" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
       <c r="Q92" s="8" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="S92" s="7" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
     </row>
     <row r="93" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="6" t="s">
-        <v>22</v>
+        <v>64</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="C93" s="8" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="D93" s="8" t="s">
-        <v>520</v>
+        <v>514</v>
       </c>
       <c r="E93" s="8" t="s">
-        <v>491</v>
+        <v>484</v>
       </c>
       <c r="F93" s="8" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="G93" s="8" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="H93" s="8" t="s">
-        <v>428</v>
+        <v>421</v>
       </c>
       <c r="K93" s="10" t="s">
-        <v>583</v>
+        <v>576</v>
       </c>
       <c r="L93" s="10" t="s">
-        <v>672</v>
+        <v>665</v>
       </c>
       <c r="M93" s="10"/>
       <c r="N93" s="10" t="s">
-        <v>459</v>
+        <v>452</v>
       </c>
       <c r="O93" s="8" t="s">
-        <v>551</v>
+        <v>544</v>
       </c>
       <c r="P93" s="8" t="s">
-        <v>396</v>
+        <v>389</v>
       </c>
       <c r="Q93" s="8" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="S93" s="7" t="s">
-        <v>364</v>
+        <v>357</v>
       </c>
     </row>
     <row r="94" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="6" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C94" s="8" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="D94" s="8" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="E94" s="8" t="s">
-        <v>492</v>
+        <v>485</v>
       </c>
       <c r="F94" s="8" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="G94" s="8" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="H94" s="8" t="s">
-        <v>429</v>
+        <v>422</v>
       </c>
       <c r="K94" s="10" t="s">
-        <v>584</v>
+        <v>577</v>
       </c>
       <c r="L94" s="10" t="s">
-        <v>673</v>
+        <v>666</v>
       </c>
       <c r="M94" s="10"/>
       <c r="N94" s="10" t="s">
-        <v>460</v>
+        <v>453</v>
       </c>
       <c r="O94" s="8" t="s">
-        <v>552</v>
+        <v>545</v>
       </c>
       <c r="P94" s="8" t="s">
-        <v>397</v>
+        <v>390</v>
       </c>
       <c r="Q94" s="8" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="S94" s="7" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
     </row>
     <row r="95" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="6" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="C95" s="8" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>522</v>
+        <v>516</v>
       </c>
       <c r="E95" s="8" t="s">
-        <v>493</v>
+        <v>486</v>
       </c>
       <c r="F95" s="8" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="G95" s="8" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="H95" s="8" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
       <c r="K95" s="10" t="s">
-        <v>585</v>
+        <v>578</v>
       </c>
       <c r="L95" s="10" t="s">
-        <v>674</v>
+        <v>667</v>
       </c>
       <c r="M95" s="10"/>
       <c r="N95" s="10" t="s">
-        <v>461</v>
+        <v>454</v>
       </c>
       <c r="O95" s="8" t="s">
-        <v>553</v>
+        <v>546</v>
       </c>
       <c r="P95" s="8" t="s">
-        <v>398</v>
+        <v>391</v>
       </c>
       <c r="Q95" s="8" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="S95" s="7" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
     </row>
     <row r="96" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="6" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="C96" s="8" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>523</v>
+        <v>517</v>
       </c>
       <c r="E96" s="8" t="s">
-        <v>493</v>
+        <v>487</v>
       </c>
       <c r="F96" s="8" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="G96" s="8" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="H96" s="8" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="K96" s="10" t="s">
-        <v>586</v>
+        <v>579</v>
       </c>
       <c r="L96" s="10" t="s">
-        <v>675</v>
+        <v>668</v>
       </c>
       <c r="M96" s="10"/>
       <c r="N96" s="10" t="s">
-        <v>462</v>
+        <v>455</v>
       </c>
       <c r="O96" s="8" t="s">
-        <v>554</v>
+        <v>547</v>
       </c>
       <c r="P96" s="8" t="s">
-        <v>399</v>
+        <v>392</v>
       </c>
       <c r="Q96" s="8" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="S96" s="7" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
     </row>
     <row r="97" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="6" t="s">
-        <v>66</v>
+        <v>20</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="C97" s="8" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>524</v>
+        <v>518</v>
       </c>
       <c r="E97" s="8" t="s">
-        <v>494</v>
+        <v>488</v>
       </c>
       <c r="F97" s="8" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="G97" s="8" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="H97" s="8" t="s">
-        <v>432</v>
+        <v>425</v>
       </c>
       <c r="K97" s="10" t="s">
-        <v>587</v>
+        <v>580</v>
       </c>
       <c r="L97" s="10" t="s">
-        <v>676</v>
+        <v>669</v>
       </c>
       <c r="M97" s="10"/>
       <c r="N97" s="10" t="s">
-        <v>463</v>
+        <v>456</v>
       </c>
       <c r="O97" s="8" t="s">
-        <v>555</v>
+        <v>548</v>
       </c>
       <c r="P97" s="8" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
       <c r="Q97" s="8" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="S97" s="7" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
     </row>
     <row r="98" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="6" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C98" s="8" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="D98" s="8" t="s">
-        <v>525</v>
+        <v>519</v>
       </c>
       <c r="E98" s="8" t="s">
-        <v>495</v>
+        <v>489</v>
       </c>
       <c r="F98" s="8" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="G98" s="8" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="H98" s="8" t="s">
-        <v>433</v>
+        <v>426</v>
       </c>
       <c r="K98" s="10" t="s">
-        <v>588</v>
+        <v>581</v>
       </c>
       <c r="L98" s="10" t="s">
-        <v>677</v>
+        <v>670</v>
       </c>
       <c r="M98" s="10"/>
       <c r="N98" s="10" t="s">
-        <v>464</v>
+        <v>457</v>
       </c>
       <c r="O98" s="8" t="s">
-        <v>556</v>
+        <v>549</v>
       </c>
       <c r="P98" s="8" t="s">
-        <v>401</v>
+        <v>394</v>
       </c>
       <c r="Q98" s="8" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="S98" s="7" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
     </row>
     <row r="99" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="6" t="s">
-        <v>27</v>
+        <v>65</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>56</v>
+        <v>275</v>
       </c>
       <c r="C99" s="8" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="D99" s="8" t="s">
-        <v>526</v>
+        <v>458</v>
       </c>
       <c r="E99" s="8" t="s">
-        <v>496</v>
+        <v>490</v>
       </c>
       <c r="F99" s="8" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="G99" s="8" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="H99" s="8" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
       <c r="K99" s="10" t="s">
-        <v>589</v>
+        <v>582</v>
       </c>
       <c r="L99" s="10" t="s">
-        <v>678</v>
+        <v>671</v>
       </c>
       <c r="M99" s="10"/>
       <c r="N99" s="10" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
       <c r="O99" s="8" t="s">
-        <v>557</v>
+        <v>550</v>
       </c>
       <c r="P99" s="8" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
       <c r="Q99" s="8" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="S99" s="7" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
     </row>
     <row r="100" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="6" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="C100" s="8" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="D100" s="8" t="s">
-        <v>527</v>
+        <v>520</v>
       </c>
       <c r="E100" s="8" t="s">
-        <v>497</v>
+        <v>491</v>
       </c>
       <c r="F100" s="8" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="G100" s="8" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="H100" s="8" t="s">
-        <v>435</v>
+        <v>428</v>
       </c>
       <c r="K100" s="10" t="s">
-        <v>590</v>
+        <v>583</v>
       </c>
       <c r="L100" s="10" t="s">
-        <v>679</v>
+        <v>672</v>
       </c>
       <c r="M100" s="10"/>
       <c r="N100" s="10" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="O100" s="8" t="s">
-        <v>558</v>
+        <v>551</v>
       </c>
       <c r="P100" s="8" t="s">
-        <v>403</v>
+        <v>396</v>
       </c>
       <c r="Q100" s="8" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="S100" s="7" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
     </row>
     <row r="101" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="6" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="C101" s="8" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="D101" s="8" t="s">
-        <v>528</v>
+        <v>521</v>
       </c>
       <c r="E101" s="8" t="s">
-        <v>498</v>
+        <v>492</v>
       </c>
       <c r="F101" s="8" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="G101" s="8" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="H101" s="8" t="s">
-        <v>436</v>
+        <v>429</v>
       </c>
       <c r="K101" s="10" t="s">
-        <v>591</v>
+        <v>584</v>
       </c>
       <c r="L101" s="10" t="s">
-        <v>680</v>
+        <v>673</v>
       </c>
       <c r="M101" s="10"/>
       <c r="N101" s="10" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
       <c r="O101" s="8" t="s">
-        <v>559</v>
+        <v>552</v>
       </c>
       <c r="P101" s="8" t="s">
-        <v>404</v>
+        <v>397</v>
       </c>
       <c r="Q101" s="8" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="S101" s="7" t="s">
-        <v>372</v>
+        <v>365</v>
       </c>
     </row>
     <row r="102" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="6" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C102" s="8" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="D102" s="8" t="s">
-        <v>529</v>
+        <v>522</v>
       </c>
       <c r="E102" s="8" t="s">
-        <v>499</v>
+        <v>493</v>
       </c>
       <c r="F102" s="8" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="G102" s="8" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="H102" s="8" t="s">
-        <v>437</v>
+        <v>430</v>
       </c>
       <c r="K102" s="10" t="s">
-        <v>592</v>
+        <v>585</v>
       </c>
       <c r="L102" s="10" t="s">
-        <v>681</v>
+        <v>674</v>
       </c>
       <c r="M102" s="10"/>
       <c r="N102" s="10" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="O102" s="8" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
       <c r="P102" s="8" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
       <c r="Q102" s="8" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="S102" s="7" t="s">
-        <v>373</v>
+        <v>366</v>
       </c>
     </row>
     <row r="103" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="6" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C103" s="8" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="D103" s="8" t="s">
-        <v>530</v>
+        <v>523</v>
       </c>
       <c r="E103" s="8" t="s">
-        <v>500</v>
+        <v>493</v>
       </c>
       <c r="F103" s="8" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="G103" s="8" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="H103" s="8" t="s">
-        <v>438</v>
+        <v>431</v>
       </c>
       <c r="K103" s="10" t="s">
-        <v>593</v>
+        <v>586</v>
       </c>
       <c r="L103" s="10" t="s">
-        <v>682</v>
+        <v>675</v>
       </c>
       <c r="M103" s="10"/>
       <c r="N103" s="10" t="s">
+        <v>462</v>
+      </c>
+      <c r="O103" s="8" t="s">
+        <v>554</v>
+      </c>
+      <c r="P103" s="8" t="s">
+        <v>399</v>
+      </c>
+      <c r="Q103" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="S103" s="7" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="104" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B104" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C104" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="D104" s="8" t="s">
+        <v>524</v>
+      </c>
+      <c r="E104" s="8" t="s">
+        <v>494</v>
+      </c>
+      <c r="F104" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="G104" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="H104" s="8" t="s">
+        <v>432</v>
+      </c>
+      <c r="K104" s="10" t="s">
+        <v>587</v>
+      </c>
+      <c r="L104" s="10" t="s">
+        <v>676</v>
+      </c>
+      <c r="M104" s="10"/>
+      <c r="N104" s="10" t="s">
+        <v>463</v>
+      </c>
+      <c r="O104" s="8" t="s">
+        <v>555</v>
+      </c>
+      <c r="P104" s="8" t="s">
+        <v>400</v>
+      </c>
+      <c r="Q104" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="S104" s="7" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="105" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B105" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C105" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="D105" s="8" t="s">
+        <v>525</v>
+      </c>
+      <c r="E105" s="8" t="s">
+        <v>495</v>
+      </c>
+      <c r="F105" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="G105" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="H105" s="8" t="s">
+        <v>433</v>
+      </c>
+      <c r="K105" s="10" t="s">
+        <v>588</v>
+      </c>
+      <c r="L105" s="10" t="s">
+        <v>677</v>
+      </c>
+      <c r="M105" s="10"/>
+      <c r="N105" s="10" t="s">
+        <v>464</v>
+      </c>
+      <c r="O105" s="8" t="s">
+        <v>556</v>
+      </c>
+      <c r="P105" s="8" t="s">
+        <v>401</v>
+      </c>
+      <c r="Q105" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="S105" s="7" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="106" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B106" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C106" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="D106" s="8" t="s">
+        <v>526</v>
+      </c>
+      <c r="E106" s="8" t="s">
+        <v>496</v>
+      </c>
+      <c r="F106" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="G106" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="H106" s="8" t="s">
+        <v>434</v>
+      </c>
+      <c r="K106" s="10" t="s">
+        <v>589</v>
+      </c>
+      <c r="L106" s="10" t="s">
+        <v>678</v>
+      </c>
+      <c r="M106" s="10"/>
+      <c r="N106" s="10" t="s">
+        <v>465</v>
+      </c>
+      <c r="O106" s="8" t="s">
+        <v>557</v>
+      </c>
+      <c r="P106" s="8" t="s">
+        <v>402</v>
+      </c>
+      <c r="Q106" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="S106" s="7" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="107" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B107" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C107" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="D107" s="8" t="s">
+        <v>527</v>
+      </c>
+      <c r="E107" s="8" t="s">
+        <v>497</v>
+      </c>
+      <c r="F107" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="G107" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="H107" s="8" t="s">
+        <v>435</v>
+      </c>
+      <c r="K107" s="10" t="s">
+        <v>590</v>
+      </c>
+      <c r="L107" s="10" t="s">
+        <v>679</v>
+      </c>
+      <c r="M107" s="10"/>
+      <c r="N107" s="10" t="s">
+        <v>466</v>
+      </c>
+      <c r="O107" s="8" t="s">
+        <v>558</v>
+      </c>
+      <c r="P107" s="8" t="s">
+        <v>403</v>
+      </c>
+      <c r="Q107" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="S107" s="7" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="108" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B108" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C108" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="D108" s="8" t="s">
+        <v>528</v>
+      </c>
+      <c r="E108" s="8" t="s">
+        <v>498</v>
+      </c>
+      <c r="F108" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="G108" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="H108" s="8" t="s">
+        <v>436</v>
+      </c>
+      <c r="K108" s="10" t="s">
+        <v>591</v>
+      </c>
+      <c r="L108" s="10" t="s">
+        <v>680</v>
+      </c>
+      <c r="M108" s="10"/>
+      <c r="N108" s="10" t="s">
+        <v>467</v>
+      </c>
+      <c r="O108" s="8" t="s">
+        <v>559</v>
+      </c>
+      <c r="P108" s="8" t="s">
+        <v>404</v>
+      </c>
+      <c r="Q108" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="S108" s="7" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="109" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B109" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C109" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="D109" s="8" t="s">
+        <v>529</v>
+      </c>
+      <c r="E109" s="8" t="s">
+        <v>499</v>
+      </c>
+      <c r="F109" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="G109" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="H109" s="8" t="s">
+        <v>437</v>
+      </c>
+      <c r="K109" s="10" t="s">
+        <v>592</v>
+      </c>
+      <c r="L109" s="10" t="s">
+        <v>681</v>
+      </c>
+      <c r="M109" s="10"/>
+      <c r="N109" s="10" t="s">
+        <v>468</v>
+      </c>
+      <c r="O109" s="8" t="s">
+        <v>560</v>
+      </c>
+      <c r="P109" s="8" t="s">
+        <v>405</v>
+      </c>
+      <c r="Q109" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="S109" s="7" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="110" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B110" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C110" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="D110" s="8" t="s">
+        <v>530</v>
+      </c>
+      <c r="E110" s="8" t="s">
+        <v>500</v>
+      </c>
+      <c r="F110" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="G110" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="H110" s="8" t="s">
+        <v>438</v>
+      </c>
+      <c r="K110" s="10" t="s">
+        <v>593</v>
+      </c>
+      <c r="L110" s="10" t="s">
+        <v>682</v>
+      </c>
+      <c r="M110" s="10"/>
+      <c r="N110" s="10" t="s">
         <v>469</v>
       </c>
-      <c r="O103" s="8" t="s">
+      <c r="O110" s="8" t="s">
         <v>561</v>
       </c>
-      <c r="P103" s="8" t="s">
+      <c r="P110" s="8" t="s">
         <v>406</v>
       </c>
-      <c r="Q103" s="8" t="s">
+      <c r="Q110" s="8" t="s">
         <v>248</v>
       </c>
-      <c r="S103" s="7" t="s">
+      <c r="S110" s="7" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="104" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A104" s="3" t="s">
+    <row r="111" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A111" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="B104" s="4" t="s">
+      <c r="B111" s="4" t="s">
         <v>273</v>
       </c>
-      <c r="C104" s="4" t="s">
+      <c r="C111" s="4" t="s">
         <v>274</v>
       </c>
-      <c r="K104" s="10"/>
-      <c r="L104" s="10"/>
-      <c r="M104" s="10"/>
-      <c r="N104" s="10"/>
+      <c r="N111" s="4" t="s">
+        <v>777</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:U1"/>

</xml_diff>

<commit_message>
Excel for item ids added and some localizations added
</commit_message>
<xml_diff>
--- a/private/INDIVIDUAL_LOCALIZATIONS_UI_1.xlsx
+++ b/private/INDIVIDUAL_LOCALIZATIONS_UI_1.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="778">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="839" uniqueCount="799">
   <si>
     <t>en_US</t>
   </si>
@@ -2361,6 +2361,69 @@
   </si>
   <si>
     <t>Pierwsza zniszczona wieża</t>
+  </si>
+  <si>
+    <t>nightMode</t>
+  </si>
+  <si>
+    <t>Night Mode</t>
+  </si>
+  <si>
+    <t>Nachtmodus</t>
+  </si>
+  <si>
+    <t>firstThreeItems</t>
+  </si>
+  <si>
+    <t>First Three Items</t>
+  </si>
+  <si>
+    <t>fourthItem</t>
+  </si>
+  <si>
+    <t>Fourth Item</t>
+  </si>
+  <si>
+    <t>fifthItem</t>
+  </si>
+  <si>
+    <t>Fifth Item</t>
+  </si>
+  <si>
+    <t>Vierter Gegenstand</t>
+  </si>
+  <si>
+    <t>Fünfter Gegenstand</t>
+  </si>
+  <si>
+    <t>Ersten Drei Gegenstände</t>
+  </si>
+  <si>
+    <t>firstTwoItems</t>
+  </si>
+  <si>
+    <t>First Two Items</t>
+  </si>
+  <si>
+    <t>Ersten Zwei Gegenstände</t>
+  </si>
+  <si>
+    <t>thirdItem</t>
+  </si>
+  <si>
+    <t>Third Item</t>
+  </si>
+  <si>
+    <t>Dritter Gegenstand</t>
+  </si>
+  <si>
+    <t>firstItem</t>
+  </si>
+  <si>
+    <t>First Item</t>
+  </si>
+  <si>
+    <t>Erster Gegenstand</t>
   </si>
 </sst>
 </file>
@@ -2823,13 +2886,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U111"/>
+  <dimension ref="A1:U118"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="L60" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B44" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N71" sqref="N71"/>
+      <selection pane="bottomRight" activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3018,363 +3081,360 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="N9" s="4" t="s">
-        <v>714</v>
+        <v>778</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>779</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>780</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>335</v>
+        <v>105</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>333</v>
+        <v>68</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>334</v>
+        <v>69</v>
       </c>
       <c r="N10" s="4" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>104</v>
+        <v>335</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>106</v>
+        <v>333</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>107</v>
+        <v>334</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>290</v>
+        <v>104</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>291</v>
+        <v>106</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>292</v>
+        <v>107</v>
       </c>
       <c r="N12" s="4" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>108</v>
+        <v>290</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>109</v>
+        <v>291</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>112</v>
+        <v>292</v>
       </c>
       <c r="N13" s="4" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N14" s="4" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>73</v>
+        <v>110</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>70</v>
+        <v>111</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>85</v>
+        <v>113</v>
       </c>
       <c r="N15" s="4" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>115</v>
+        <v>73</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>114</v>
+        <v>70</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>118</v>
+        <v>85</v>
       </c>
       <c r="N16" s="4" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="N17" s="4" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>293</v>
+        <v>116</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>296</v>
+        <v>117</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>301</v>
+        <v>119</v>
       </c>
       <c r="N18" s="4" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="N19" s="4" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>320</v>
+        <v>294</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>321</v>
+        <v>295</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>322</v>
+        <v>300</v>
       </c>
       <c r="N20" s="4" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>298</v>
+        <v>320</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>297</v>
+        <v>321</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>299</v>
+        <v>322</v>
       </c>
       <c r="N21" s="4" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>622</v>
+        <v>298</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>620</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>621</v>
+        <v>297</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>299</v>
       </c>
       <c r="N22" s="4" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>623</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>624</v>
+        <v>622</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>620</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="N23" s="4" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>640</v>
+        <v>624</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>640</v>
+        <v>625</v>
       </c>
       <c r="N24" s="4" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>638</v>
+        <v>640</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="N25" s="4" t="s">
-        <v>638</v>
+        <v>729</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>628</v>
+        <v>638</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>637</v>
+        <v>639</v>
       </c>
       <c r="N26" s="4" t="s">
-        <v>730</v>
+        <v>638</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>635</v>
+        <v>628</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="N27" s="4" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>641</v>
+        <v>635</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>642</v>
+        <v>636</v>
       </c>
       <c r="N28" s="4" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>633</v>
+        <v>641</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>634</v>
+        <v>642</v>
       </c>
       <c r="N29" s="4" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>643</v>
+        <v>632</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>644</v>
+        <v>633</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>647</v>
+        <v>634</v>
       </c>
       <c r="N30" s="4" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="N31" s="4" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>86</v>
+        <v>645</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>646</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>648</v>
       </c>
       <c r="N32" s="4" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="N33" s="4" t="s">
-        <v>75</v>
+        <v>736</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>75</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="N34" s="4" t="s">
         <v>75</v>
@@ -3382,2223 +3442,2321 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N35" s="4" t="s">
-        <v>737</v>
+        <v>75</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="N36" s="4" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>249</v>
+        <v>82</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>250</v>
+        <v>83</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>251</v>
+        <v>84</v>
       </c>
       <c r="N37" s="4" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>342</v>
+        <v>251</v>
       </c>
       <c r="N38" s="4" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>255</v>
+        <v>342</v>
       </c>
       <c r="N39" s="4" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>319</v>
+        <v>255</v>
       </c>
       <c r="N40" s="4" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>261</v>
+        <v>269</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>262</v>
+        <v>319</v>
       </c>
       <c r="N41" s="4" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="N42" s="4" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>310</v>
+        <v>258</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>313</v>
+        <v>259</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>318</v>
+        <v>260</v>
       </c>
       <c r="N43" s="4" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="N44" s="4" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="N45" s="4" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>265</v>
+        <v>312</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>266</v>
+        <v>315</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>267</v>
+        <v>316</v>
       </c>
       <c r="N46" s="4" t="s">
-        <v>745</v>
+        <v>747</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>649</v>
-      </c>
-      <c r="B47" s="9" t="s">
-        <v>650</v>
-      </c>
-      <c r="C47" s="9" t="s">
-        <v>651</v>
+        <v>265</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>267</v>
       </c>
       <c r="N47" s="4" t="s">
-        <v>748</v>
+        <v>745</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>268</v>
+        <v>649</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>650</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>651</v>
       </c>
       <c r="N48" s="4" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>283</v>
+        <v>263</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>284</v>
+        <v>264</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>285</v>
+        <v>268</v>
       </c>
       <c r="N49" s="4" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>276</v>
+        <v>283</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>277</v>
+        <v>284</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>278</v>
+        <v>285</v>
       </c>
       <c r="N50" s="4" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="N51" s="4" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>683</v>
-      </c>
-      <c r="B52" s="9" t="s">
-        <v>684</v>
-      </c>
-      <c r="C52" s="9" t="s">
-        <v>684</v>
+        <v>279</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>280</v>
       </c>
       <c r="N52" s="4" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>282</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>282</v>
+        <v>683</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>684</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>684</v>
       </c>
       <c r="N53" s="4" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>302</v>
+        <v>281</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>303</v>
+        <v>282</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>303</v>
+        <v>282</v>
       </c>
       <c r="N54" s="4" t="s">
-        <v>303</v>
+        <v>754</v>
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="N55" s="4" t="s">
-        <v>755</v>
+        <v>303</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="N56" s="4" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>323</v>
+        <v>307</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>328</v>
+        <v>308</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>309</v>
       </c>
       <c r="N57" s="4" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="N58" s="4" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="N59" s="4" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="N60" s="4" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="N61" s="4" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>336</v>
+        <v>326</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>337</v>
-      </c>
-      <c r="C62" s="4" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="N62" s="4" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>687</v>
-      </c>
-      <c r="B63" s="9" t="s">
-        <v>688</v>
-      </c>
-      <c r="C63" s="9" t="s">
-        <v>689</v>
+        <v>336</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>338</v>
       </c>
       <c r="N63" s="4" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
+        <v>687</v>
+      </c>
+      <c r="B64" s="9" t="s">
+        <v>688</v>
+      </c>
+      <c r="C64" s="9" t="s">
+        <v>689</v>
+      </c>
+      <c r="N64" s="4" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
         <v>690</v>
       </c>
-      <c r="B64" s="9" t="s">
+      <c r="B65" s="9" t="s">
         <v>691</v>
       </c>
-      <c r="C64" s="9" t="s">
+      <c r="C65" s="9" t="s">
         <v>692</v>
       </c>
-      <c r="N64" s="4" t="s">
+      <c r="N65" s="4" t="s">
         <v>764</v>
       </c>
     </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A65" s="3" t="s">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A66" s="3" t="s">
         <v>339</v>
       </c>
-      <c r="B65" s="4" t="s">
+      <c r="B66" s="4" t="s">
         <v>340</v>
       </c>
-      <c r="C65" s="4" t="s">
+      <c r="C66" s="4" t="s">
         <v>341</v>
-      </c>
-      <c r="J65" s="5"/>
-      <c r="K65" s="5"/>
-      <c r="N65" s="4" t="s">
-        <v>765</v>
-      </c>
-      <c r="O65" s="5"/>
-    </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A66" s="3" t="s">
-        <v>612</v>
-      </c>
-      <c r="B66" s="4" t="s">
-        <v>613</v>
-      </c>
-      <c r="C66" s="4" t="s">
-        <v>614</v>
       </c>
       <c r="J66" s="5"/>
       <c r="K66" s="5"/>
       <c r="N66" s="4" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="O66" s="5"/>
     </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>606</v>
+        <v>612</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>609</v>
-      </c>
-      <c r="C67" s="9" t="s">
-        <v>609</v>
+        <v>613</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>614</v>
       </c>
       <c r="J67" s="5"/>
       <c r="K67" s="5"/>
       <c r="N67" s="4" t="s">
+        <v>766</v>
+      </c>
+      <c r="O67" s="5"/>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A68" s="3" t="s">
+        <v>606</v>
+      </c>
+      <c r="B68" s="4" t="s">
         <v>609</v>
       </c>
-      <c r="O67" s="5"/>
-    </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A68" s="3" t="s">
-        <v>607</v>
-      </c>
-      <c r="B68" s="4" t="s">
-        <v>610</v>
-      </c>
       <c r="C68" s="9" t="s">
-        <v>615</v>
+        <v>609</v>
       </c>
       <c r="J68" s="5"/>
       <c r="K68" s="5"/>
       <c r="N68" s="4" t="s">
-        <v>767</v>
+        <v>609</v>
       </c>
       <c r="O68" s="5"/>
     </row>
-    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="J69" s="5"/>
       <c r="K69" s="5"/>
       <c r="N69" s="4" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="O69" s="5"/>
     </row>
-    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>696</v>
-      </c>
-      <c r="B70" s="9" t="s">
-        <v>698</v>
+        <v>608</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>611</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>700</v>
+        <v>616</v>
       </c>
       <c r="J70" s="5"/>
       <c r="K70" s="5"/>
       <c r="N70" s="4" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="O70" s="5"/>
     </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="J71" s="5"/>
       <c r="K71" s="5"/>
       <c r="N71" s="4" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="O71" s="5"/>
     </row>
-    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>693</v>
+        <v>697</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>694</v>
+        <v>699</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>695</v>
+        <v>701</v>
       </c>
       <c r="J72" s="5"/>
       <c r="K72" s="5"/>
       <c r="N72" s="4" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="O72" s="5"/>
     </row>
-    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
-        <v>702</v>
+        <v>693</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>703</v>
+        <v>694</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>704</v>
+        <v>695</v>
       </c>
       <c r="J73" s="5"/>
       <c r="K73" s="5"/>
       <c r="N73" s="4" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="O73" s="5"/>
     </row>
-    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>707</v>
+        <v>704</v>
       </c>
       <c r="J74" s="5"/>
       <c r="K74" s="5"/>
       <c r="N74" s="4" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="O74" s="5"/>
     </row>
-    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
-        <v>617</v>
+        <v>705</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>618</v>
+        <v>706</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>619</v>
+        <v>707</v>
       </c>
       <c r="J75" s="5"/>
       <c r="K75" s="5"/>
       <c r="N75" s="4" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="O75" s="5"/>
     </row>
-    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
-        <v>600</v>
-      </c>
-      <c r="B76" s="4" t="s">
-        <v>603</v>
-      </c>
-      <c r="C76" s="4" t="s">
-        <v>604</v>
+        <v>796</v>
+      </c>
+      <c r="B76" s="9" t="s">
+        <v>797</v>
+      </c>
+      <c r="C76" s="9" t="s">
+        <v>798</v>
       </c>
       <c r="J76" s="5"/>
       <c r="K76" s="5"/>
-      <c r="N76" s="4" t="s">
+      <c r="O76" s="5"/>
+    </row>
+    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A77" s="3" t="s">
+        <v>790</v>
+      </c>
+      <c r="B77" s="9" t="s">
+        <v>791</v>
+      </c>
+      <c r="C77" s="9" t="s">
+        <v>792</v>
+      </c>
+      <c r="J77" s="5"/>
+      <c r="K77" s="5"/>
+      <c r="O77" s="5"/>
+    </row>
+    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A78" s="3" t="s">
+        <v>781</v>
+      </c>
+      <c r="B78" s="9" t="s">
+        <v>782</v>
+      </c>
+      <c r="C78" s="9" t="s">
+        <v>789</v>
+      </c>
+      <c r="J78" s="5"/>
+      <c r="K78" s="5"/>
+      <c r="O78" s="5"/>
+    </row>
+    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A79" s="3" t="s">
+        <v>793</v>
+      </c>
+      <c r="B79" s="9" t="s">
+        <v>794</v>
+      </c>
+      <c r="C79" s="9" t="s">
+        <v>795</v>
+      </c>
+      <c r="J79" s="5"/>
+      <c r="K79" s="5"/>
+      <c r="O79" s="5"/>
+    </row>
+    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A80" s="3" t="s">
+        <v>783</v>
+      </c>
+      <c r="B80" s="9" t="s">
+        <v>784</v>
+      </c>
+      <c r="C80" s="9" t="s">
+        <v>787</v>
+      </c>
+      <c r="J80" s="5"/>
+      <c r="K80" s="5"/>
+      <c r="O80" s="5"/>
+    </row>
+    <row r="81" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A81" s="3" t="s">
+        <v>785</v>
+      </c>
+      <c r="B81" s="9" t="s">
+        <v>786</v>
+      </c>
+      <c r="C81" s="9" t="s">
+        <v>788</v>
+      </c>
+      <c r="J81" s="5"/>
+      <c r="K81" s="5"/>
+      <c r="O81" s="5"/>
+    </row>
+    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A82" s="3" t="s">
+        <v>617</v>
+      </c>
+      <c r="B82" s="9" t="s">
+        <v>618</v>
+      </c>
+      <c r="C82" s="9" t="s">
+        <v>619</v>
+      </c>
+      <c r="J82" s="5"/>
+      <c r="K82" s="5"/>
+      <c r="N82" s="4" t="s">
+        <v>774</v>
+      </c>
+      <c r="O82" s="5"/>
+    </row>
+    <row r="83" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A83" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="B83" s="4" t="s">
+        <v>603</v>
+      </c>
+      <c r="C83" s="4" t="s">
+        <v>604</v>
+      </c>
+      <c r="J83" s="5"/>
+      <c r="K83" s="5"/>
+      <c r="N83" s="4" t="s">
         <v>775</v>
       </c>
-      <c r="O76" s="5"/>
-    </row>
-    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A77" s="3" t="s">
+      <c r="O83" s="5"/>
+    </row>
+    <row r="84" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A84" s="3" t="s">
         <v>601</v>
       </c>
-      <c r="B77" s="4" t="s">
+      <c r="B84" s="4" t="s">
         <v>602</v>
       </c>
-      <c r="C77" s="4" t="s">
+      <c r="C84" s="4" t="s">
         <v>605</v>
       </c>
-      <c r="N77" s="4" t="s">
+      <c r="N84" s="4" t="s">
         <v>776</v>
       </c>
-      <c r="O77" s="5"/>
-    </row>
-    <row r="78" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B78" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C78" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="D78" s="8" t="s">
-        <v>501</v>
-      </c>
-      <c r="E78" s="8" t="s">
-        <v>470</v>
-      </c>
-      <c r="F78" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="G78" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="H78" s="8" t="s">
-        <v>407</v>
-      </c>
-      <c r="K78" s="10" t="s">
-        <v>562</v>
-      </c>
-      <c r="L78" s="10" t="s">
-        <v>652</v>
-      </c>
-      <c r="M78" s="10"/>
-      <c r="N78" s="10" t="s">
-        <v>439</v>
-      </c>
-      <c r="O78" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="P78" s="8" t="s">
-        <v>375</v>
-      </c>
-      <c r="Q78" s="8" t="s">
-        <v>217</v>
-      </c>
-      <c r="S78" s="7" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="79" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B79" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C79" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D79" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E79" s="8" t="s">
-        <v>471</v>
-      </c>
-      <c r="F79" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="G79" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="H79" s="8" t="s">
-        <v>408</v>
-      </c>
-      <c r="K79" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="L79" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="M79" s="10"/>
-      <c r="N79" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="O79" s="8" t="s">
-        <v>531</v>
-      </c>
-      <c r="P79" s="8" t="s">
-        <v>376</v>
-      </c>
-      <c r="Q79" s="8" t="s">
-        <v>218</v>
-      </c>
-      <c r="S79" s="7" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="80" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B80" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C80" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="D80" s="8" t="s">
-        <v>502</v>
-      </c>
-      <c r="E80" s="8" t="s">
-        <v>472</v>
-      </c>
-      <c r="F80" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="G80" s="8" t="s">
-        <v>187</v>
-      </c>
-      <c r="H80" s="8" t="s">
-        <v>409</v>
-      </c>
-      <c r="K80" s="10" t="s">
-        <v>563</v>
-      </c>
-      <c r="L80" s="10" t="s">
-        <v>653</v>
-      </c>
-      <c r="M80" s="10"/>
-      <c r="N80" s="10" t="s">
-        <v>440</v>
-      </c>
-      <c r="O80" s="8" t="s">
-        <v>532</v>
-      </c>
-      <c r="P80" s="8" t="s">
-        <v>377</v>
-      </c>
-      <c r="Q80" s="8" t="s">
-        <v>219</v>
-      </c>
-      <c r="S80" s="7" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="81" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B81" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C81" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="D81" s="8" t="s">
-        <v>503</v>
-      </c>
-      <c r="E81" s="8" t="s">
-        <v>473</v>
-      </c>
-      <c r="F81" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="G81" s="8" t="s">
-        <v>188</v>
-      </c>
-      <c r="H81" s="8" t="s">
-        <v>410</v>
-      </c>
-      <c r="K81" s="10" t="s">
-        <v>564</v>
-      </c>
-      <c r="L81" s="10" t="s">
-        <v>654</v>
-      </c>
-      <c r="M81" s="10"/>
-      <c r="N81" s="10" t="s">
-        <v>441</v>
-      </c>
-      <c r="O81" s="8" t="s">
-        <v>533</v>
-      </c>
-      <c r="P81" s="8" t="s">
-        <v>378</v>
-      </c>
-      <c r="Q81" s="8" t="s">
-        <v>220</v>
-      </c>
-      <c r="S81" s="7" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="82" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B82" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C82" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="D82" s="8" t="s">
-        <v>504</v>
-      </c>
-      <c r="E82" s="8" t="s">
-        <v>474</v>
-      </c>
-      <c r="F82" s="8" t="s">
-        <v>159</v>
-      </c>
-      <c r="G82" s="8" t="s">
-        <v>189</v>
-      </c>
-      <c r="H82" s="8" t="s">
-        <v>411</v>
-      </c>
-      <c r="K82" s="10" t="s">
-        <v>565</v>
-      </c>
-      <c r="L82" s="10" t="s">
-        <v>655</v>
-      </c>
-      <c r="M82" s="10"/>
-      <c r="N82" s="10" t="s">
-        <v>442</v>
-      </c>
-      <c r="O82" s="8" t="s">
-        <v>534</v>
-      </c>
-      <c r="P82" s="8" t="s">
-        <v>379</v>
-      </c>
-      <c r="Q82" s="8" t="s">
-        <v>221</v>
-      </c>
-      <c r="S82" s="7" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="83" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="B83" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="C83" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="D83" s="8" t="s">
-        <v>505</v>
-      </c>
-      <c r="E83" s="8" t="s">
-        <v>475</v>
-      </c>
-      <c r="F83" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="G83" s="8" t="s">
-        <v>190</v>
-      </c>
-      <c r="H83" s="8" t="s">
-        <v>412</v>
-      </c>
-      <c r="K83" s="10" t="s">
-        <v>566</v>
-      </c>
-      <c r="L83" s="10" t="s">
-        <v>656</v>
-      </c>
-      <c r="M83" s="10"/>
-      <c r="N83" s="10" t="s">
-        <v>443</v>
-      </c>
-      <c r="O83" s="8" t="s">
-        <v>535</v>
-      </c>
-      <c r="P83" s="8" t="s">
-        <v>380</v>
-      </c>
-      <c r="Q83" s="8" t="s">
-        <v>222</v>
-      </c>
-      <c r="S83" s="7" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="84" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B84" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C84" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="D84" s="8" t="s">
-        <v>506</v>
-      </c>
-      <c r="E84" s="8" t="s">
-        <v>476</v>
-      </c>
-      <c r="F84" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="G84" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="H84" s="8" t="s">
-        <v>413</v>
-      </c>
-      <c r="K84" s="10" t="s">
-        <v>567</v>
-      </c>
-      <c r="L84" s="10" t="s">
-        <v>657</v>
-      </c>
-      <c r="M84" s="10"/>
-      <c r="N84" s="10" t="s">
-        <v>444</v>
-      </c>
-      <c r="O84" s="8" t="s">
-        <v>536</v>
-      </c>
-      <c r="P84" s="8" t="s">
-        <v>381</v>
-      </c>
-      <c r="Q84" s="8" t="s">
-        <v>223</v>
-      </c>
-      <c r="S84" s="7" t="s">
-        <v>349</v>
-      </c>
+      <c r="O84" s="5"/>
     </row>
     <row r="85" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="6" t="s">
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="C85" s="8" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="D85" s="8" t="s">
-        <v>507</v>
+        <v>501</v>
       </c>
       <c r="E85" s="8" t="s">
-        <v>477</v>
+        <v>470</v>
       </c>
       <c r="F85" s="8" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="G85" s="8" t="s">
-        <v>192</v>
+        <v>60</v>
       </c>
       <c r="H85" s="8" t="s">
-        <v>414</v>
+        <v>407</v>
       </c>
       <c r="K85" s="10" t="s">
-        <v>568</v>
+        <v>562</v>
       </c>
       <c r="L85" s="10" t="s">
-        <v>658</v>
+        <v>652</v>
       </c>
       <c r="M85" s="10"/>
       <c r="N85" s="10" t="s">
-        <v>445</v>
+        <v>439</v>
       </c>
       <c r="O85" s="8" t="s">
-        <v>537</v>
+        <v>155</v>
       </c>
       <c r="P85" s="8" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="Q85" s="8" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="S85" s="7" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
     </row>
     <row r="86" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="C86" s="8" t="s">
-        <v>133</v>
+        <v>7</v>
       </c>
       <c r="D86" s="8" t="s">
-        <v>508</v>
+        <v>7</v>
       </c>
       <c r="E86" s="8" t="s">
-        <v>478</v>
+        <v>471</v>
       </c>
       <c r="F86" s="8" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="G86" s="8" t="s">
-        <v>193</v>
+        <v>7</v>
       </c>
       <c r="H86" s="8" t="s">
-        <v>415</v>
+        <v>408</v>
       </c>
       <c r="K86" s="10" t="s">
-        <v>569</v>
+        <v>7</v>
       </c>
       <c r="L86" s="10" t="s">
-        <v>659</v>
+        <v>7</v>
       </c>
       <c r="M86" s="10"/>
       <c r="N86" s="10" t="s">
-        <v>446</v>
+        <v>7</v>
       </c>
       <c r="O86" s="8" t="s">
-        <v>538</v>
+        <v>531</v>
       </c>
       <c r="P86" s="8" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="Q86" s="8" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="S86" s="7" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
     </row>
     <row r="87" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="6" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C87" s="8" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="D87" s="8" t="s">
-        <v>509</v>
+        <v>502</v>
       </c>
       <c r="E87" s="8" t="s">
-        <v>479</v>
+        <v>472</v>
       </c>
       <c r="F87" s="8" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="G87" s="8" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="H87" s="8" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
       <c r="K87" s="10" t="s">
-        <v>570</v>
+        <v>563</v>
       </c>
       <c r="L87" s="10" t="s">
-        <v>660</v>
+        <v>653</v>
       </c>
       <c r="M87" s="10"/>
       <c r="N87" s="10" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
       <c r="O87" s="8" t="s">
-        <v>539</v>
+        <v>532</v>
       </c>
       <c r="P87" s="8" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="Q87" s="8" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="S87" s="7" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
     </row>
     <row r="88" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="6" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C88" s="8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D88" s="8" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="E88" s="8" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="F88" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G88" s="8" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H88" s="8" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="K88" s="10" t="s">
-        <v>571</v>
+        <v>564</v>
       </c>
       <c r="L88" s="10" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="M88" s="10"/>
       <c r="N88" s="10" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="O88" s="8" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="P88" s="8" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="Q88" s="8" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="S88" s="7" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="89" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="6" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C89" s="8" t="s">
-        <v>271</v>
+        <v>129</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>510</v>
+        <v>504</v>
       </c>
       <c r="E89" s="8" t="s">
-        <v>480</v>
+        <v>474</v>
       </c>
       <c r="F89" s="8" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="G89" s="8" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="H89" s="8" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
       <c r="K89" s="10" t="s">
-        <v>572</v>
+        <v>565</v>
       </c>
       <c r="L89" s="10" t="s">
-        <v>661</v>
+        <v>655</v>
       </c>
       <c r="M89" s="10"/>
       <c r="N89" s="10" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="O89" s="8" t="s">
-        <v>540</v>
+        <v>534</v>
       </c>
       <c r="P89" s="8" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
       <c r="Q89" s="8" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="S89" s="7" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
     </row>
     <row r="90" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="6" t="s">
-        <v>14</v>
+        <v>62</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="C90" s="8" t="s">
-        <v>270</v>
+        <v>130</v>
       </c>
       <c r="D90" s="8" t="s">
-        <v>511</v>
+        <v>505</v>
       </c>
       <c r="E90" s="8" t="s">
-        <v>481</v>
+        <v>475</v>
       </c>
       <c r="F90" s="8" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="G90" s="8" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="H90" s="8" t="s">
-        <v>418</v>
+        <v>412</v>
       </c>
       <c r="K90" s="10" t="s">
-        <v>573</v>
+        <v>566</v>
       </c>
       <c r="L90" s="10" t="s">
-        <v>662</v>
+        <v>656</v>
       </c>
       <c r="M90" s="10"/>
       <c r="N90" s="10" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="O90" s="8" t="s">
-        <v>541</v>
+        <v>535</v>
       </c>
       <c r="P90" s="8" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="Q90" s="8" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="S90" s="7" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
     </row>
     <row r="91" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="6" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="C91" s="8" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D91" s="8" t="s">
-        <v>512</v>
+        <v>506</v>
       </c>
       <c r="E91" s="8" t="s">
-        <v>482</v>
+        <v>476</v>
       </c>
       <c r="F91" s="8" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="G91" s="8" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="H91" s="8" t="s">
-        <v>419</v>
+        <v>413</v>
       </c>
       <c r="K91" s="10" t="s">
-        <v>574</v>
+        <v>567</v>
       </c>
       <c r="L91" s="10" t="s">
-        <v>663</v>
+        <v>657</v>
       </c>
       <c r="M91" s="10"/>
       <c r="N91" s="10" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="O91" s="8" t="s">
-        <v>542</v>
+        <v>536</v>
       </c>
       <c r="P91" s="8" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="Q91" s="8" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="S91" s="7" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
     </row>
     <row r="92" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="6" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C92" s="8" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D92" s="8" t="s">
-        <v>513</v>
+        <v>507</v>
       </c>
       <c r="E92" s="8" t="s">
-        <v>483</v>
+        <v>477</v>
       </c>
       <c r="F92" s="8" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="G92" s="8" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="H92" s="8" t="s">
-        <v>420</v>
+        <v>414</v>
       </c>
       <c r="K92" s="10" t="s">
-        <v>575</v>
+        <v>568</v>
       </c>
       <c r="L92" s="10" t="s">
-        <v>664</v>
+        <v>658</v>
       </c>
       <c r="M92" s="10"/>
       <c r="N92" s="10" t="s">
-        <v>451</v>
+        <v>445</v>
       </c>
       <c r="O92" s="8" t="s">
-        <v>543</v>
+        <v>537</v>
       </c>
       <c r="P92" s="8" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="Q92" s="8" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="S92" s="7" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
     </row>
     <row r="93" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="6" t="s">
-        <v>64</v>
+        <v>10</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="C93" s="8" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D93" s="8" t="s">
-        <v>514</v>
+        <v>508</v>
       </c>
       <c r="E93" s="8" t="s">
-        <v>484</v>
+        <v>478</v>
       </c>
       <c r="F93" s="8" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="G93" s="8" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="H93" s="8" t="s">
-        <v>421</v>
+        <v>415</v>
       </c>
       <c r="K93" s="10" t="s">
-        <v>576</v>
+        <v>569</v>
       </c>
       <c r="L93" s="10" t="s">
-        <v>665</v>
+        <v>659</v>
       </c>
       <c r="M93" s="10"/>
       <c r="N93" s="10" t="s">
-        <v>452</v>
+        <v>446</v>
       </c>
       <c r="O93" s="8" t="s">
-        <v>544</v>
+        <v>538</v>
       </c>
       <c r="P93" s="8" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
       <c r="Q93" s="8" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="S93" s="7" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
     </row>
     <row r="94" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="6" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C94" s="8" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D94" s="8" t="s">
-        <v>515</v>
+        <v>509</v>
       </c>
       <c r="E94" s="8" t="s">
-        <v>485</v>
+        <v>479</v>
       </c>
       <c r="F94" s="8" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="G94" s="8" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="H94" s="8" t="s">
-        <v>422</v>
+        <v>416</v>
       </c>
       <c r="K94" s="10" t="s">
-        <v>577</v>
+        <v>570</v>
       </c>
       <c r="L94" s="10" t="s">
-        <v>666</v>
+        <v>660</v>
       </c>
       <c r="M94" s="10"/>
       <c r="N94" s="10" t="s">
-        <v>453</v>
+        <v>447</v>
       </c>
       <c r="O94" s="8" t="s">
-        <v>545</v>
+        <v>539</v>
       </c>
       <c r="P94" s="8" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="Q94" s="8" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="S94" s="7" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
     </row>
     <row r="95" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="6" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C95" s="8" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>516</v>
+        <v>505</v>
       </c>
       <c r="E95" s="8" t="s">
-        <v>486</v>
+        <v>475</v>
       </c>
       <c r="F95" s="8" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="G95" s="8" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="H95" s="8" t="s">
-        <v>423</v>
+        <v>412</v>
       </c>
       <c r="K95" s="10" t="s">
-        <v>578</v>
+        <v>571</v>
       </c>
       <c r="L95" s="10" t="s">
-        <v>667</v>
+        <v>656</v>
       </c>
       <c r="M95" s="10"/>
       <c r="N95" s="10" t="s">
-        <v>454</v>
+        <v>443</v>
       </c>
       <c r="O95" s="8" t="s">
-        <v>546</v>
+        <v>535</v>
       </c>
       <c r="P95" s="8" t="s">
-        <v>391</v>
+        <v>380</v>
       </c>
       <c r="Q95" s="8" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
       <c r="S95" s="7" t="s">
-        <v>359</v>
+        <v>348</v>
       </c>
     </row>
     <row r="96" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="6" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C96" s="8" t="s">
-        <v>140</v>
+        <v>271</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>517</v>
+        <v>510</v>
       </c>
       <c r="E96" s="8" t="s">
-        <v>487</v>
+        <v>480</v>
       </c>
       <c r="F96" s="8" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="G96" s="8" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="H96" s="8" t="s">
-        <v>424</v>
+        <v>417</v>
       </c>
       <c r="K96" s="10" t="s">
-        <v>579</v>
+        <v>572</v>
       </c>
       <c r="L96" s="10" t="s">
-        <v>668</v>
+        <v>661</v>
       </c>
       <c r="M96" s="10"/>
       <c r="N96" s="10" t="s">
-        <v>455</v>
+        <v>448</v>
       </c>
       <c r="O96" s="8" t="s">
-        <v>547</v>
+        <v>540</v>
       </c>
       <c r="P96" s="8" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
       <c r="Q96" s="8" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="S96" s="7" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
     </row>
     <row r="97" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="6" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C97" s="8" t="s">
-        <v>141</v>
+        <v>270</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>518</v>
+        <v>511</v>
       </c>
       <c r="E97" s="8" t="s">
-        <v>488</v>
+        <v>481</v>
       </c>
       <c r="F97" s="8" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="G97" s="8" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="H97" s="8" t="s">
-        <v>425</v>
+        <v>418</v>
       </c>
       <c r="K97" s="10" t="s">
-        <v>580</v>
+        <v>573</v>
       </c>
       <c r="L97" s="10" t="s">
-        <v>669</v>
+        <v>662</v>
       </c>
       <c r="M97" s="10"/>
       <c r="N97" s="10" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
       <c r="O97" s="8" t="s">
-        <v>548</v>
+        <v>541</v>
       </c>
       <c r="P97" s="8" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="Q97" s="8" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="S97" s="7" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
     </row>
     <row r="98" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C98" s="8" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="D98" s="8" t="s">
-        <v>519</v>
+        <v>512</v>
       </c>
       <c r="E98" s="8" t="s">
-        <v>489</v>
+        <v>482</v>
       </c>
       <c r="F98" s="8" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="G98" s="8" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="H98" s="8" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
       <c r="K98" s="10" t="s">
-        <v>581</v>
+        <v>574</v>
       </c>
       <c r="L98" s="10" t="s">
-        <v>670</v>
+        <v>663</v>
       </c>
       <c r="M98" s="10"/>
       <c r="N98" s="10" t="s">
-        <v>457</v>
+        <v>450</v>
       </c>
       <c r="O98" s="8" t="s">
-        <v>549</v>
+        <v>542</v>
       </c>
       <c r="P98" s="8" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
       <c r="Q98" s="8" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="S98" s="7" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
     </row>
     <row r="99" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="6" t="s">
-        <v>65</v>
+        <v>16</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>275</v>
+        <v>39</v>
       </c>
       <c r="C99" s="8" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="D99" s="8" t="s">
-        <v>458</v>
+        <v>513</v>
       </c>
       <c r="E99" s="8" t="s">
-        <v>490</v>
+        <v>483</v>
       </c>
       <c r="F99" s="8" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="G99" s="8" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="H99" s="8" t="s">
-        <v>427</v>
+        <v>420</v>
       </c>
       <c r="K99" s="10" t="s">
-        <v>582</v>
+        <v>575</v>
       </c>
       <c r="L99" s="10" t="s">
-        <v>671</v>
+        <v>664</v>
       </c>
       <c r="M99" s="10"/>
       <c r="N99" s="10" t="s">
-        <v>458</v>
+        <v>451</v>
       </c>
       <c r="O99" s="8" t="s">
-        <v>550</v>
+        <v>543</v>
       </c>
       <c r="P99" s="8" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
       <c r="Q99" s="8" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="S99" s="7" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
     </row>
     <row r="100" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="6" t="s">
-        <v>22</v>
+        <v>64</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="C100" s="8" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="D100" s="8" t="s">
-        <v>520</v>
+        <v>514</v>
       </c>
       <c r="E100" s="8" t="s">
-        <v>491</v>
+        <v>484</v>
       </c>
       <c r="F100" s="8" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="G100" s="8" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="H100" s="8" t="s">
-        <v>428</v>
+        <v>421</v>
       </c>
       <c r="K100" s="10" t="s">
-        <v>583</v>
+        <v>576</v>
       </c>
       <c r="L100" s="10" t="s">
-        <v>672</v>
+        <v>665</v>
       </c>
       <c r="M100" s="10"/>
       <c r="N100" s="10" t="s">
-        <v>459</v>
+        <v>452</v>
       </c>
       <c r="O100" s="8" t="s">
-        <v>551</v>
+        <v>544</v>
       </c>
       <c r="P100" s="8" t="s">
-        <v>396</v>
+        <v>389</v>
       </c>
       <c r="Q100" s="8" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="S100" s="7" t="s">
-        <v>364</v>
+        <v>357</v>
       </c>
     </row>
     <row r="101" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="6" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C101" s="8" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="D101" s="8" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="E101" s="8" t="s">
-        <v>492</v>
+        <v>485</v>
       </c>
       <c r="F101" s="8" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="G101" s="8" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="H101" s="8" t="s">
-        <v>429</v>
+        <v>422</v>
       </c>
       <c r="K101" s="10" t="s">
-        <v>584</v>
+        <v>577</v>
       </c>
       <c r="L101" s="10" t="s">
-        <v>673</v>
+        <v>666</v>
       </c>
       <c r="M101" s="10"/>
       <c r="N101" s="10" t="s">
-        <v>460</v>
+        <v>453</v>
       </c>
       <c r="O101" s="8" t="s">
-        <v>552</v>
+        <v>545</v>
       </c>
       <c r="P101" s="8" t="s">
-        <v>397</v>
+        <v>390</v>
       </c>
       <c r="Q101" s="8" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="S101" s="7" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
     </row>
     <row r="102" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="6" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="C102" s="8" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="D102" s="8" t="s">
-        <v>522</v>
+        <v>516</v>
       </c>
       <c r="E102" s="8" t="s">
-        <v>493</v>
+        <v>486</v>
       </c>
       <c r="F102" s="8" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="G102" s="8" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="H102" s="8" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
       <c r="K102" s="10" t="s">
-        <v>585</v>
+        <v>578</v>
       </c>
       <c r="L102" s="10" t="s">
-        <v>674</v>
+        <v>667</v>
       </c>
       <c r="M102" s="10"/>
       <c r="N102" s="10" t="s">
-        <v>461</v>
+        <v>454</v>
       </c>
       <c r="O102" s="8" t="s">
-        <v>553</v>
+        <v>546</v>
       </c>
       <c r="P102" s="8" t="s">
-        <v>398</v>
+        <v>391</v>
       </c>
       <c r="Q102" s="8" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="S102" s="7" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
     </row>
     <row r="103" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="6" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="C103" s="8" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="D103" s="8" t="s">
-        <v>523</v>
+        <v>517</v>
       </c>
       <c r="E103" s="8" t="s">
-        <v>493</v>
+        <v>487</v>
       </c>
       <c r="F103" s="8" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="G103" s="8" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="H103" s="8" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="K103" s="10" t="s">
-        <v>586</v>
+        <v>579</v>
       </c>
       <c r="L103" s="10" t="s">
-        <v>675</v>
+        <v>668</v>
       </c>
       <c r="M103" s="10"/>
       <c r="N103" s="10" t="s">
-        <v>462</v>
+        <v>455</v>
       </c>
       <c r="O103" s="8" t="s">
-        <v>554</v>
+        <v>547</v>
       </c>
       <c r="P103" s="8" t="s">
-        <v>399</v>
+        <v>392</v>
       </c>
       <c r="Q103" s="8" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="S103" s="7" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
     </row>
     <row r="104" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="6" t="s">
-        <v>66</v>
+        <v>20</v>
       </c>
       <c r="B104" s="7" t="s">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="C104" s="8" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="D104" s="8" t="s">
-        <v>524</v>
+        <v>518</v>
       </c>
       <c r="E104" s="8" t="s">
-        <v>494</v>
+        <v>488</v>
       </c>
       <c r="F104" s="8" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="G104" s="8" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="H104" s="8" t="s">
-        <v>432</v>
+        <v>425</v>
       </c>
       <c r="K104" s="10" t="s">
-        <v>587</v>
+        <v>580</v>
       </c>
       <c r="L104" s="10" t="s">
-        <v>676</v>
+        <v>669</v>
       </c>
       <c r="M104" s="10"/>
       <c r="N104" s="10" t="s">
-        <v>463</v>
+        <v>456</v>
       </c>
       <c r="O104" s="8" t="s">
-        <v>555</v>
+        <v>548</v>
       </c>
       <c r="P104" s="8" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
       <c r="Q104" s="8" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="S104" s="7" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
     </row>
     <row r="105" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="6" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B105" s="7" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C105" s="8" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="D105" s="8" t="s">
-        <v>525</v>
+        <v>519</v>
       </c>
       <c r="E105" s="8" t="s">
-        <v>495</v>
+        <v>489</v>
       </c>
       <c r="F105" s="8" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="G105" s="8" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="H105" s="8" t="s">
-        <v>433</v>
+        <v>426</v>
       </c>
       <c r="K105" s="10" t="s">
-        <v>588</v>
+        <v>581</v>
       </c>
       <c r="L105" s="10" t="s">
-        <v>677</v>
+        <v>670</v>
       </c>
       <c r="M105" s="10"/>
       <c r="N105" s="10" t="s">
-        <v>464</v>
+        <v>457</v>
       </c>
       <c r="O105" s="8" t="s">
-        <v>556</v>
+        <v>549</v>
       </c>
       <c r="P105" s="8" t="s">
-        <v>401</v>
+        <v>394</v>
       </c>
       <c r="Q105" s="8" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="S105" s="7" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
     </row>
     <row r="106" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="6" t="s">
-        <v>27</v>
+        <v>65</v>
       </c>
       <c r="B106" s="7" t="s">
-        <v>56</v>
+        <v>275</v>
       </c>
       <c r="C106" s="8" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="D106" s="8" t="s">
-        <v>526</v>
+        <v>458</v>
       </c>
       <c r="E106" s="8" t="s">
-        <v>496</v>
+        <v>490</v>
       </c>
       <c r="F106" s="8" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="G106" s="8" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="H106" s="8" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
       <c r="K106" s="10" t="s">
-        <v>589</v>
+        <v>582</v>
       </c>
       <c r="L106" s="10" t="s">
-        <v>678</v>
+        <v>671</v>
       </c>
       <c r="M106" s="10"/>
       <c r="N106" s="10" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
       <c r="O106" s="8" t="s">
-        <v>557</v>
+        <v>550</v>
       </c>
       <c r="P106" s="8" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
       <c r="Q106" s="8" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="S106" s="7" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
     </row>
     <row r="107" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="6" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="C107" s="8" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="D107" s="8" t="s">
-        <v>527</v>
+        <v>520</v>
       </c>
       <c r="E107" s="8" t="s">
-        <v>497</v>
+        <v>491</v>
       </c>
       <c r="F107" s="8" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="G107" s="8" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="H107" s="8" t="s">
-        <v>435</v>
+        <v>428</v>
       </c>
       <c r="K107" s="10" t="s">
-        <v>590</v>
+        <v>583</v>
       </c>
       <c r="L107" s="10" t="s">
-        <v>679</v>
+        <v>672</v>
       </c>
       <c r="M107" s="10"/>
       <c r="N107" s="10" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="O107" s="8" t="s">
-        <v>558</v>
+        <v>551</v>
       </c>
       <c r="P107" s="8" t="s">
-        <v>403</v>
+        <v>396</v>
       </c>
       <c r="Q107" s="8" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="S107" s="7" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
     </row>
     <row r="108" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="6" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="C108" s="8" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="D108" s="8" t="s">
-        <v>528</v>
+        <v>521</v>
       </c>
       <c r="E108" s="8" t="s">
-        <v>498</v>
+        <v>492</v>
       </c>
       <c r="F108" s="8" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="G108" s="8" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="H108" s="8" t="s">
-        <v>436</v>
+        <v>429</v>
       </c>
       <c r="K108" s="10" t="s">
-        <v>591</v>
+        <v>584</v>
       </c>
       <c r="L108" s="10" t="s">
-        <v>680</v>
+        <v>673</v>
       </c>
       <c r="M108" s="10"/>
       <c r="N108" s="10" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
       <c r="O108" s="8" t="s">
-        <v>559</v>
+        <v>552</v>
       </c>
       <c r="P108" s="8" t="s">
-        <v>404</v>
+        <v>397</v>
       </c>
       <c r="Q108" s="8" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="S108" s="7" t="s">
-        <v>372</v>
+        <v>365</v>
       </c>
     </row>
     <row r="109" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="6" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C109" s="8" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="D109" s="8" t="s">
-        <v>529</v>
+        <v>522</v>
       </c>
       <c r="E109" s="8" t="s">
-        <v>499</v>
+        <v>493</v>
       </c>
       <c r="F109" s="8" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="G109" s="8" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="H109" s="8" t="s">
-        <v>437</v>
+        <v>430</v>
       </c>
       <c r="K109" s="10" t="s">
-        <v>592</v>
+        <v>585</v>
       </c>
       <c r="L109" s="10" t="s">
-        <v>681</v>
+        <v>674</v>
       </c>
       <c r="M109" s="10"/>
       <c r="N109" s="10" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="O109" s="8" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
       <c r="P109" s="8" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
       <c r="Q109" s="8" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="S109" s="7" t="s">
-        <v>373</v>
+        <v>366</v>
       </c>
     </row>
     <row r="110" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="6" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B110" s="7" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C110" s="8" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="D110" s="8" t="s">
-        <v>530</v>
+        <v>523</v>
       </c>
       <c r="E110" s="8" t="s">
-        <v>500</v>
+        <v>493</v>
       </c>
       <c r="F110" s="8" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="G110" s="8" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="H110" s="8" t="s">
-        <v>438</v>
+        <v>431</v>
       </c>
       <c r="K110" s="10" t="s">
-        <v>593</v>
+        <v>586</v>
       </c>
       <c r="L110" s="10" t="s">
-        <v>682</v>
+        <v>675</v>
       </c>
       <c r="M110" s="10"/>
       <c r="N110" s="10" t="s">
+        <v>462</v>
+      </c>
+      <c r="O110" s="8" t="s">
+        <v>554</v>
+      </c>
+      <c r="P110" s="8" t="s">
+        <v>399</v>
+      </c>
+      <c r="Q110" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="S110" s="7" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="111" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B111" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C111" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="D111" s="8" t="s">
+        <v>524</v>
+      </c>
+      <c r="E111" s="8" t="s">
+        <v>494</v>
+      </c>
+      <c r="F111" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="G111" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="H111" s="8" t="s">
+        <v>432</v>
+      </c>
+      <c r="K111" s="10" t="s">
+        <v>587</v>
+      </c>
+      <c r="L111" s="10" t="s">
+        <v>676</v>
+      </c>
+      <c r="M111" s="10"/>
+      <c r="N111" s="10" t="s">
+        <v>463</v>
+      </c>
+      <c r="O111" s="8" t="s">
+        <v>555</v>
+      </c>
+      <c r="P111" s="8" t="s">
+        <v>400</v>
+      </c>
+      <c r="Q111" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="S111" s="7" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="112" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B112" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C112" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="D112" s="8" t="s">
+        <v>525</v>
+      </c>
+      <c r="E112" s="8" t="s">
+        <v>495</v>
+      </c>
+      <c r="F112" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="G112" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="H112" s="8" t="s">
+        <v>433</v>
+      </c>
+      <c r="K112" s="10" t="s">
+        <v>588</v>
+      </c>
+      <c r="L112" s="10" t="s">
+        <v>677</v>
+      </c>
+      <c r="M112" s="10"/>
+      <c r="N112" s="10" t="s">
+        <v>464</v>
+      </c>
+      <c r="O112" s="8" t="s">
+        <v>556</v>
+      </c>
+      <c r="P112" s="8" t="s">
+        <v>401</v>
+      </c>
+      <c r="Q112" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="S112" s="7" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="113" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B113" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C113" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="D113" s="8" t="s">
+        <v>526</v>
+      </c>
+      <c r="E113" s="8" t="s">
+        <v>496</v>
+      </c>
+      <c r="F113" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="G113" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="H113" s="8" t="s">
+        <v>434</v>
+      </c>
+      <c r="K113" s="10" t="s">
+        <v>589</v>
+      </c>
+      <c r="L113" s="10" t="s">
+        <v>678</v>
+      </c>
+      <c r="M113" s="10"/>
+      <c r="N113" s="10" t="s">
+        <v>465</v>
+      </c>
+      <c r="O113" s="8" t="s">
+        <v>557</v>
+      </c>
+      <c r="P113" s="8" t="s">
+        <v>402</v>
+      </c>
+      <c r="Q113" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="S113" s="7" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="114" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B114" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C114" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="D114" s="8" t="s">
+        <v>527</v>
+      </c>
+      <c r="E114" s="8" t="s">
+        <v>497</v>
+      </c>
+      <c r="F114" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="G114" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="H114" s="8" t="s">
+        <v>435</v>
+      </c>
+      <c r="K114" s="10" t="s">
+        <v>590</v>
+      </c>
+      <c r="L114" s="10" t="s">
+        <v>679</v>
+      </c>
+      <c r="M114" s="10"/>
+      <c r="N114" s="10" t="s">
+        <v>466</v>
+      </c>
+      <c r="O114" s="8" t="s">
+        <v>558</v>
+      </c>
+      <c r="P114" s="8" t="s">
+        <v>403</v>
+      </c>
+      <c r="Q114" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="S114" s="7" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="115" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B115" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C115" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="D115" s="8" t="s">
+        <v>528</v>
+      </c>
+      <c r="E115" s="8" t="s">
+        <v>498</v>
+      </c>
+      <c r="F115" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="G115" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="H115" s="8" t="s">
+        <v>436</v>
+      </c>
+      <c r="K115" s="10" t="s">
+        <v>591</v>
+      </c>
+      <c r="L115" s="10" t="s">
+        <v>680</v>
+      </c>
+      <c r="M115" s="10"/>
+      <c r="N115" s="10" t="s">
+        <v>467</v>
+      </c>
+      <c r="O115" s="8" t="s">
+        <v>559</v>
+      </c>
+      <c r="P115" s="8" t="s">
+        <v>404</v>
+      </c>
+      <c r="Q115" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="S115" s="7" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="116" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B116" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C116" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="D116" s="8" t="s">
+        <v>529</v>
+      </c>
+      <c r="E116" s="8" t="s">
+        <v>499</v>
+      </c>
+      <c r="F116" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="G116" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="H116" s="8" t="s">
+        <v>437</v>
+      </c>
+      <c r="K116" s="10" t="s">
+        <v>592</v>
+      </c>
+      <c r="L116" s="10" t="s">
+        <v>681</v>
+      </c>
+      <c r="M116" s="10"/>
+      <c r="N116" s="10" t="s">
+        <v>468</v>
+      </c>
+      <c r="O116" s="8" t="s">
+        <v>560</v>
+      </c>
+      <c r="P116" s="8" t="s">
+        <v>405</v>
+      </c>
+      <c r="Q116" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="S116" s="7" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="117" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B117" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C117" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="D117" s="8" t="s">
+        <v>530</v>
+      </c>
+      <c r="E117" s="8" t="s">
+        <v>500</v>
+      </c>
+      <c r="F117" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="G117" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="H117" s="8" t="s">
+        <v>438</v>
+      </c>
+      <c r="K117" s="10" t="s">
+        <v>593</v>
+      </c>
+      <c r="L117" s="10" t="s">
+        <v>682</v>
+      </c>
+      <c r="M117" s="10"/>
+      <c r="N117" s="10" t="s">
         <v>469</v>
       </c>
-      <c r="O110" s="8" t="s">
+      <c r="O117" s="8" t="s">
         <v>561</v>
       </c>
-      <c r="P110" s="8" t="s">
+      <c r="P117" s="8" t="s">
         <v>406</v>
       </c>
-      <c r="Q110" s="8" t="s">
+      <c r="Q117" s="8" t="s">
         <v>248</v>
       </c>
-      <c r="S110" s="7" t="s">
+      <c r="S117" s="7" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="111" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A111" s="3" t="s">
+    <row r="118" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A118" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="B111" s="4" t="s">
+      <c r="B118" s="4" t="s">
         <v>273</v>
       </c>
-      <c r="C111" s="4" t="s">
+      <c r="C118" s="4" t="s">
         <v>274</v>
       </c>
-      <c r="N111" s="4" t="s">
+      <c r="N118" s="4" t="s">
         <v>777</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update localization excel and items excel
</commit_message>
<xml_diff>
--- a/private/INDIVIDUAL_LOCALIZATIONS_UI_1.xlsx
+++ b/private/INDIVIDUAL_LOCALIZATIONS_UI_1.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -15,7 +15,7 @@
     <sheet name="INTL" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">INTL!$A$1:$U$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">INTL!$A$1:$U$127</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="839" uniqueCount="799">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="867" uniqueCount="825">
   <si>
     <t>en_US</t>
   </si>
@@ -2424,6 +2424,84 @@
   </si>
   <si>
     <t>Erster Gegenstand</t>
+  </si>
+  <si>
+    <t>excludeRegions</t>
+  </si>
+  <si>
+    <t>Exclude regions</t>
+  </si>
+  <si>
+    <t>Regionen ausschließen</t>
+  </si>
+  <si>
+    <t>regionEuropeWest</t>
+  </si>
+  <si>
+    <t>regionKorea</t>
+  </si>
+  <si>
+    <t>regionNorthAmerica</t>
+  </si>
+  <si>
+    <t>North America</t>
+  </si>
+  <si>
+    <t>Nordamerika</t>
+  </si>
+  <si>
+    <t>Korea</t>
+  </si>
+  <si>
+    <t>Europe West</t>
+  </si>
+  <si>
+    <t>Westeuropa</t>
+  </si>
+  <si>
+    <t>playedBy</t>
+  </si>
+  <si>
+    <t>Played By</t>
+  </si>
+  <si>
+    <t>Gespielt Von</t>
+  </si>
+  <si>
+    <t>starterTrinket</t>
+  </si>
+  <si>
+    <t>Starter Trinket</t>
+  </si>
+  <si>
+    <t>Starttrinket</t>
+  </si>
+  <si>
+    <t>goToMatch</t>
+  </si>
+  <si>
+    <t>Go to Match</t>
+  </si>
+  <si>
+    <t>Gehe zu Match</t>
+  </si>
+  <si>
+    <t>noFeaturedMatchFoundWithUsedCriterias</t>
+  </si>
+  <si>
+    <t>No Featured Match found with the used criterias!</t>
+  </si>
+  <si>
+    <t>Keine Ausgewähltes Match mit den genutzen Kriterien gefunden!</t>
+  </si>
+  <si>
+    <t>target</t>
+  </si>
+  <si>
+    <t>Target</t>
+  </si>
+  <si>
+    <t>Ziel</t>
   </si>
 </sst>
 </file>
@@ -2886,13 +2964,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U118"/>
+  <dimension ref="A1:U127"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B44" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B58" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B75" sqref="B75"/>
+      <selection pane="bottomRight" activeCell="A80" sqref="A80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3092,1008 +3170,981 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="N10" s="4" t="s">
-        <v>714</v>
+        <v>799</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>800</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>801</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>335</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>333</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>334</v>
-      </c>
-      <c r="N11" s="4" t="s">
-        <v>715</v>
+        <v>802</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>808</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>809</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="N12" s="4" t="s">
-        <v>716</v>
+        <v>803</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>807</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>807</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>290</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>292</v>
-      </c>
-      <c r="N13" s="4" t="s">
-        <v>717</v>
+        <v>804</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>805</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>806</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>109</v>
+        <v>68</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>112</v>
+        <v>69</v>
       </c>
       <c r="N14" s="4" t="s">
-        <v>718</v>
+        <v>714</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>110</v>
+        <v>335</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>111</v>
+        <v>333</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>113</v>
+        <v>334</v>
       </c>
       <c r="N15" s="4" t="s">
-        <v>719</v>
+        <v>715</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>73</v>
+        <v>104</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>70</v>
+        <v>106</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>85</v>
+        <v>107</v>
       </c>
       <c r="N16" s="4" t="s">
-        <v>720</v>
+        <v>716</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>115</v>
+        <v>290</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>114</v>
+        <v>291</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>118</v>
+        <v>292</v>
       </c>
       <c r="N17" s="4" t="s">
-        <v>721</v>
+        <v>717</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="N18" s="4" t="s">
-        <v>722</v>
+        <v>718</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>293</v>
+        <v>110</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>296</v>
+        <v>111</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>301</v>
+        <v>113</v>
       </c>
       <c r="N19" s="4" t="s">
-        <v>723</v>
+        <v>719</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>294</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>295</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>300</v>
+        <v>819</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>820</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>821</v>
       </c>
       <c r="N20" s="4" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>320</v>
+        <v>73</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>321</v>
+        <v>70</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>322</v>
+        <v>85</v>
       </c>
       <c r="N21" s="4" t="s">
-        <v>725</v>
+        <v>720</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>298</v>
+        <v>115</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>297</v>
+        <v>114</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>299</v>
+        <v>118</v>
       </c>
       <c r="N22" s="4" t="s">
-        <v>726</v>
+        <v>721</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>622</v>
+        <v>116</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>620</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>621</v>
+        <v>117</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>119</v>
       </c>
       <c r="N23" s="4" t="s">
-        <v>727</v>
+        <v>722</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>623</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>624</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>625</v>
+        <v>293</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>301</v>
       </c>
       <c r="N24" s="4" t="s">
-        <v>728</v>
+        <v>723</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>626</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>640</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>640</v>
+        <v>294</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>300</v>
       </c>
       <c r="N25" s="4" t="s">
-        <v>729</v>
+        <v>724</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>627</v>
-      </c>
-      <c r="B26" s="9" t="s">
-        <v>638</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>639</v>
+        <v>320</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>322</v>
       </c>
       <c r="N26" s="4" t="s">
-        <v>638</v>
+        <v>725</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>629</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>628</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>637</v>
+        <v>298</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>299</v>
       </c>
       <c r="N27" s="4" t="s">
-        <v>730</v>
+        <v>726</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>630</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>635</v>
+        <v>622</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>620</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>636</v>
+        <v>621</v>
       </c>
       <c r="N28" s="4" t="s">
-        <v>731</v>
+        <v>727</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>631</v>
+        <v>623</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>641</v>
+        <v>624</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>642</v>
+        <v>625</v>
       </c>
       <c r="N29" s="4" t="s">
-        <v>732</v>
+        <v>728</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>632</v>
+        <v>626</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>633</v>
+        <v>640</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>634</v>
+        <v>640</v>
       </c>
       <c r="N30" s="4" t="s">
-        <v>733</v>
+        <v>729</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>643</v>
+        <v>627</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>644</v>
+        <v>638</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>647</v>
+        <v>639</v>
       </c>
       <c r="N31" s="4" t="s">
-        <v>734</v>
+        <v>638</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>645</v>
+        <v>629</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>646</v>
+        <v>628</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>648</v>
+        <v>637</v>
       </c>
       <c r="N32" s="4" t="s">
-        <v>735</v>
+        <v>730</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>86</v>
+        <v>630</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>635</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>636</v>
       </c>
       <c r="N33" s="4" t="s">
-        <v>736</v>
+        <v>731</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>76</v>
+        <v>631</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>641</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>642</v>
       </c>
       <c r="N34" s="4" t="s">
-        <v>75</v>
+        <v>732</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>80</v>
+        <v>632</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>633</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>634</v>
       </c>
       <c r="N35" s="4" t="s">
-        <v>75</v>
+        <v>733</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>81</v>
+        <v>643</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>644</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>647</v>
       </c>
       <c r="N36" s="4" t="s">
-        <v>737</v>
+        <v>734</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>84</v>
+        <v>645</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>646</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>648</v>
       </c>
       <c r="N37" s="4" t="s">
-        <v>738</v>
+        <v>735</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>249</v>
+        <v>72</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>250</v>
+        <v>71</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>251</v>
+        <v>86</v>
       </c>
       <c r="N38" s="4" t="s">
-        <v>739</v>
+        <v>736</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>252</v>
+        <v>74</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>253</v>
+        <v>75</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>342</v>
+        <v>76</v>
       </c>
       <c r="N39" s="4" t="s">
-        <v>740</v>
+        <v>75</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>254</v>
+        <v>77</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>255</v>
+        <v>75</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>255</v>
+        <v>80</v>
       </c>
       <c r="N40" s="4" t="s">
-        <v>741</v>
+        <v>75</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>256</v>
+        <v>78</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>269</v>
+        <v>79</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>319</v>
+        <v>81</v>
       </c>
       <c r="N41" s="4" t="s">
-        <v>742</v>
+        <v>737</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>257</v>
+        <v>82</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>261</v>
+        <v>83</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>262</v>
+        <v>84</v>
       </c>
       <c r="N42" s="4" t="s">
-        <v>743</v>
+        <v>738</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>259</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>260</v>
-      </c>
-      <c r="N43" s="4" t="s">
-        <v>744</v>
+        <v>816</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>817</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>818</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>310</v>
+        <v>249</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>313</v>
+        <v>250</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>318</v>
+        <v>251</v>
       </c>
       <c r="N44" s="4" t="s">
-        <v>745</v>
+        <v>739</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>311</v>
+        <v>252</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>314</v>
+        <v>253</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>317</v>
+        <v>342</v>
       </c>
       <c r="N45" s="4" t="s">
-        <v>746</v>
+        <v>740</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>312</v>
+        <v>254</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>315</v>
+        <v>255</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>316</v>
+        <v>255</v>
       </c>
       <c r="N46" s="4" t="s">
-        <v>747</v>
+        <v>741</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>267</v>
+        <v>319</v>
       </c>
       <c r="N47" s="4" t="s">
-        <v>745</v>
+        <v>742</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>649</v>
-      </c>
-      <c r="B48" s="9" t="s">
-        <v>650</v>
-      </c>
-      <c r="C48" s="9" t="s">
-        <v>651</v>
+        <v>257</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>262</v>
       </c>
       <c r="N48" s="4" t="s">
-        <v>748</v>
+        <v>743</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="N49" s="4" t="s">
-        <v>749</v>
+        <v>744</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>284</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>285</v>
-      </c>
-      <c r="N50" s="4" t="s">
-        <v>750</v>
+        <v>810</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>811</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>812</v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>276</v>
+        <v>310</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>277</v>
+        <v>313</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>278</v>
+        <v>318</v>
       </c>
       <c r="N51" s="4" t="s">
-        <v>751</v>
+        <v>745</v>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>279</v>
+        <v>311</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>280</v>
+        <v>314</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>280</v>
+        <v>317</v>
       </c>
       <c r="N52" s="4" t="s">
-        <v>752</v>
+        <v>746</v>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>683</v>
-      </c>
-      <c r="B53" s="9" t="s">
-        <v>684</v>
-      </c>
-      <c r="C53" s="9" t="s">
-        <v>684</v>
+        <v>312</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>316</v>
       </c>
       <c r="N53" s="4" t="s">
-        <v>753</v>
+        <v>747</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>282</v>
+        <v>267</v>
       </c>
       <c r="N54" s="4" t="s">
-        <v>754</v>
+        <v>745</v>
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>302</v>
-      </c>
-      <c r="B55" s="4" t="s">
-        <v>303</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>303</v>
+        <v>649</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>650</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>651</v>
       </c>
       <c r="N55" s="4" t="s">
-        <v>303</v>
+        <v>748</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>304</v>
+        <v>263</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>305</v>
+        <v>264</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>306</v>
+        <v>268</v>
       </c>
       <c r="N56" s="4" t="s">
-        <v>755</v>
+        <v>749</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>307</v>
+        <v>283</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>308</v>
+        <v>284</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>309</v>
+        <v>285</v>
       </c>
       <c r="N57" s="4" t="s">
-        <v>756</v>
+        <v>750</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>323</v>
+        <v>276</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>328</v>
+        <v>277</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>278</v>
       </c>
       <c r="N58" s="4" t="s">
-        <v>757</v>
+        <v>751</v>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>327</v>
+        <v>279</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>329</v>
+        <v>280</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>280</v>
       </c>
       <c r="N59" s="4" t="s">
-        <v>758</v>
+        <v>752</v>
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>324</v>
-      </c>
-      <c r="B60" s="4" t="s">
-        <v>330</v>
+        <v>683</v>
+      </c>
+      <c r="B60" s="9" t="s">
+        <v>684</v>
+      </c>
+      <c r="C60" s="9" t="s">
+        <v>684</v>
       </c>
       <c r="N60" s="4" t="s">
-        <v>759</v>
+        <v>753</v>
       </c>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>325</v>
+        <v>281</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>332</v>
+        <v>282</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>282</v>
       </c>
       <c r="N61" s="4" t="s">
-        <v>760</v>
+        <v>754</v>
       </c>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>326</v>
+        <v>302</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>331</v>
+        <v>303</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>303</v>
       </c>
       <c r="N62" s="4" t="s">
-        <v>761</v>
+        <v>303</v>
       </c>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>336</v>
+        <v>304</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>337</v>
+        <v>305</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>338</v>
+        <v>306</v>
       </c>
       <c r="N63" s="4" t="s">
-        <v>762</v>
+        <v>755</v>
       </c>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>687</v>
-      </c>
-      <c r="B64" s="9" t="s">
-        <v>688</v>
-      </c>
-      <c r="C64" s="9" t="s">
-        <v>689</v>
+        <v>307</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>309</v>
       </c>
       <c r="N64" s="4" t="s">
-        <v>763</v>
+        <v>756</v>
       </c>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>690</v>
-      </c>
-      <c r="B65" s="9" t="s">
-        <v>691</v>
-      </c>
-      <c r="C65" s="9" t="s">
-        <v>692</v>
+        <v>323</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>328</v>
       </c>
       <c r="N65" s="4" t="s">
-        <v>764</v>
+        <v>757</v>
       </c>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>339</v>
+        <v>327</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>340</v>
-      </c>
-      <c r="C66" s="4" t="s">
-        <v>341</v>
-      </c>
-      <c r="J66" s="5"/>
-      <c r="K66" s="5"/>
+        <v>329</v>
+      </c>
       <c r="N66" s="4" t="s">
-        <v>765</v>
-      </c>
-      <c r="O66" s="5"/>
+        <v>758</v>
+      </c>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>612</v>
+        <v>324</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>613</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>614</v>
-      </c>
-      <c r="J67" s="5"/>
-      <c r="K67" s="5"/>
+        <v>330</v>
+      </c>
       <c r="N67" s="4" t="s">
-        <v>766</v>
-      </c>
-      <c r="O67" s="5"/>
+        <v>759</v>
+      </c>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>606</v>
+        <v>325</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>609</v>
-      </c>
-      <c r="C68" s="9" t="s">
-        <v>609</v>
-      </c>
-      <c r="J68" s="5"/>
-      <c r="K68" s="5"/>
+        <v>332</v>
+      </c>
       <c r="N68" s="4" t="s">
-        <v>609</v>
-      </c>
-      <c r="O68" s="5"/>
+        <v>760</v>
+      </c>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>607</v>
+        <v>326</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>610</v>
-      </c>
-      <c r="C69" s="9" t="s">
-        <v>615</v>
-      </c>
-      <c r="J69" s="5"/>
-      <c r="K69" s="5"/>
+        <v>331</v>
+      </c>
       <c r="N69" s="4" t="s">
-        <v>767</v>
-      </c>
-      <c r="O69" s="5"/>
+        <v>761</v>
+      </c>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>608</v>
+        <v>336</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>611</v>
-      </c>
-      <c r="C70" s="9" t="s">
-        <v>616</v>
-      </c>
-      <c r="J70" s="5"/>
-      <c r="K70" s="5"/>
+        <v>337</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>338</v>
+      </c>
       <c r="N70" s="4" t="s">
-        <v>768</v>
-      </c>
-      <c r="O70" s="5"/>
+        <v>762</v>
+      </c>
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>696</v>
+        <v>687</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>698</v>
+        <v>688</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>700</v>
-      </c>
-      <c r="J71" s="5"/>
-      <c r="K71" s="5"/>
+        <v>689</v>
+      </c>
       <c r="N71" s="4" t="s">
-        <v>769</v>
-      </c>
-      <c r="O71" s="5"/>
+        <v>763</v>
+      </c>
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>697</v>
+        <v>690</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>699</v>
+        <v>691</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>701</v>
-      </c>
-      <c r="J72" s="5"/>
-      <c r="K72" s="5"/>
+        <v>692</v>
+      </c>
       <c r="N72" s="4" t="s">
-        <v>770</v>
-      </c>
-      <c r="O72" s="5"/>
+        <v>764</v>
+      </c>
     </row>
     <row r="73" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
-        <v>693</v>
-      </c>
-      <c r="B73" s="9" t="s">
-        <v>694</v>
-      </c>
-      <c r="C73" s="9" t="s">
-        <v>695</v>
+        <v>339</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>341</v>
       </c>
       <c r="J73" s="5"/>
       <c r="K73" s="5"/>
       <c r="N73" s="4" t="s">
-        <v>771</v>
+        <v>765</v>
       </c>
       <c r="O73" s="5"/>
     </row>
     <row r="74" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
-        <v>702</v>
-      </c>
-      <c r="B74" s="9" t="s">
-        <v>703</v>
-      </c>
-      <c r="C74" s="9" t="s">
-        <v>704</v>
+        <v>612</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>613</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>614</v>
       </c>
       <c r="J74" s="5"/>
       <c r="K74" s="5"/>
       <c r="N74" s="4" t="s">
-        <v>772</v>
+        <v>766</v>
       </c>
       <c r="O74" s="5"/>
     </row>
     <row r="75" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
-        <v>705</v>
-      </c>
-      <c r="B75" s="9" t="s">
-        <v>706</v>
+        <v>606</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>609</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>707</v>
+        <v>609</v>
       </c>
       <c r="J75" s="5"/>
       <c r="K75" s="5"/>
       <c r="N75" s="4" t="s">
-        <v>773</v>
+        <v>609</v>
       </c>
       <c r="O75" s="5"/>
     </row>
     <row r="76" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
-        <v>796</v>
-      </c>
-      <c r="B76" s="9" t="s">
-        <v>797</v>
+        <v>607</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>610</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>798</v>
+        <v>615</v>
       </c>
       <c r="J76" s="5"/>
       <c r="K76" s="5"/>
+      <c r="N76" s="4" t="s">
+        <v>767</v>
+      </c>
       <c r="O76" s="5"/>
     </row>
     <row r="77" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
-        <v>790</v>
-      </c>
-      <c r="B77" s="9" t="s">
-        <v>791</v>
+        <v>608</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>611</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>792</v>
+        <v>616</v>
       </c>
       <c r="J77" s="5"/>
       <c r="K77" s="5"/>
+      <c r="N77" s="4" t="s">
+        <v>768</v>
+      </c>
       <c r="O77" s="5"/>
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
-        <v>781</v>
+        <v>696</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>782</v>
+        <v>698</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>789</v>
+        <v>700</v>
       </c>
       <c r="J78" s="5"/>
       <c r="K78" s="5"/>
+      <c r="N78" s="4" t="s">
+        <v>769</v>
+      </c>
       <c r="O78" s="5"/>
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>793</v>
+        <v>697</v>
       </c>
       <c r="B79" s="9" t="s">
-        <v>794</v>
+        <v>699</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>795</v>
+        <v>701</v>
       </c>
       <c r="J79" s="5"/>
       <c r="K79" s="5"/>
+      <c r="N79" s="4" t="s">
+        <v>770</v>
+      </c>
       <c r="O79" s="5"/>
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
-        <v>783</v>
+        <v>822</v>
       </c>
       <c r="B80" s="9" t="s">
-        <v>784</v>
+        <v>823</v>
       </c>
       <c r="C80" s="9" t="s">
-        <v>787</v>
+        <v>824</v>
       </c>
       <c r="J80" s="5"/>
       <c r="K80" s="5"/>
@@ -4101,1667 +4152,1802 @@
     </row>
     <row r="81" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
-        <v>785</v>
+        <v>693</v>
       </c>
       <c r="B81" s="9" t="s">
-        <v>786</v>
+        <v>694</v>
       </c>
       <c r="C81" s="9" t="s">
-        <v>788</v>
+        <v>695</v>
       </c>
       <c r="J81" s="5"/>
       <c r="K81" s="5"/>
+      <c r="N81" s="4" t="s">
+        <v>771</v>
+      </c>
       <c r="O81" s="5"/>
     </row>
     <row r="82" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
-        <v>617</v>
+        <v>813</v>
       </c>
       <c r="B82" s="9" t="s">
-        <v>618</v>
+        <v>814</v>
       </c>
       <c r="C82" s="9" t="s">
-        <v>619</v>
+        <v>815</v>
       </c>
       <c r="J82" s="5"/>
       <c r="K82" s="5"/>
-      <c r="N82" s="4" t="s">
-        <v>774</v>
-      </c>
       <c r="O82" s="5"/>
     </row>
     <row r="83" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
-        <v>600</v>
-      </c>
-      <c r="B83" s="4" t="s">
-        <v>603</v>
-      </c>
-      <c r="C83" s="4" t="s">
-        <v>604</v>
+        <v>702</v>
+      </c>
+      <c r="B83" s="9" t="s">
+        <v>703</v>
+      </c>
+      <c r="C83" s="9" t="s">
+        <v>704</v>
       </c>
       <c r="J83" s="5"/>
       <c r="K83" s="5"/>
       <c r="N83" s="4" t="s">
-        <v>775</v>
+        <v>772</v>
       </c>
       <c r="O83" s="5"/>
     </row>
     <row r="84" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
+        <v>705</v>
+      </c>
+      <c r="B84" s="9" t="s">
+        <v>706</v>
+      </c>
+      <c r="C84" s="9" t="s">
+        <v>707</v>
+      </c>
+      <c r="J84" s="5"/>
+      <c r="K84" s="5"/>
+      <c r="N84" s="4" t="s">
+        <v>773</v>
+      </c>
+      <c r="O84" s="5"/>
+    </row>
+    <row r="85" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A85" s="3" t="s">
+        <v>796</v>
+      </c>
+      <c r="B85" s="9" t="s">
+        <v>797</v>
+      </c>
+      <c r="C85" s="9" t="s">
+        <v>798</v>
+      </c>
+      <c r="J85" s="5"/>
+      <c r="K85" s="5"/>
+      <c r="O85" s="5"/>
+    </row>
+    <row r="86" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A86" s="3" t="s">
+        <v>790</v>
+      </c>
+      <c r="B86" s="9" t="s">
+        <v>791</v>
+      </c>
+      <c r="C86" s="9" t="s">
+        <v>792</v>
+      </c>
+      <c r="J86" s="5"/>
+      <c r="K86" s="5"/>
+      <c r="O86" s="5"/>
+    </row>
+    <row r="87" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A87" s="3" t="s">
+        <v>781</v>
+      </c>
+      <c r="B87" s="9" t="s">
+        <v>782</v>
+      </c>
+      <c r="C87" s="9" t="s">
+        <v>789</v>
+      </c>
+      <c r="J87" s="5"/>
+      <c r="K87" s="5"/>
+      <c r="O87" s="5"/>
+    </row>
+    <row r="88" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A88" s="3" t="s">
+        <v>793</v>
+      </c>
+      <c r="B88" s="9" t="s">
+        <v>794</v>
+      </c>
+      <c r="C88" s="9" t="s">
+        <v>795</v>
+      </c>
+      <c r="J88" s="5"/>
+      <c r="K88" s="5"/>
+      <c r="O88" s="5"/>
+    </row>
+    <row r="89" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A89" s="3" t="s">
+        <v>783</v>
+      </c>
+      <c r="B89" s="9" t="s">
+        <v>784</v>
+      </c>
+      <c r="C89" s="9" t="s">
+        <v>787</v>
+      </c>
+      <c r="J89" s="5"/>
+      <c r="K89" s="5"/>
+      <c r="O89" s="5"/>
+    </row>
+    <row r="90" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A90" s="3" t="s">
+        <v>785</v>
+      </c>
+      <c r="B90" s="9" t="s">
+        <v>786</v>
+      </c>
+      <c r="C90" s="9" t="s">
+        <v>788</v>
+      </c>
+      <c r="J90" s="5"/>
+      <c r="K90" s="5"/>
+      <c r="O90" s="5"/>
+    </row>
+    <row r="91" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A91" s="3" t="s">
+        <v>617</v>
+      </c>
+      <c r="B91" s="9" t="s">
+        <v>618</v>
+      </c>
+      <c r="C91" s="9" t="s">
+        <v>619</v>
+      </c>
+      <c r="J91" s="5"/>
+      <c r="K91" s="5"/>
+      <c r="N91" s="4" t="s">
+        <v>774</v>
+      </c>
+      <c r="O91" s="5"/>
+    </row>
+    <row r="92" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A92" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="B92" s="4" t="s">
+        <v>603</v>
+      </c>
+      <c r="C92" s="4" t="s">
+        <v>604</v>
+      </c>
+      <c r="J92" s="5"/>
+      <c r="K92" s="5"/>
+      <c r="N92" s="4" t="s">
+        <v>775</v>
+      </c>
+      <c r="O92" s="5"/>
+    </row>
+    <row r="93" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A93" s="3" t="s">
         <v>601</v>
       </c>
-      <c r="B84" s="4" t="s">
+      <c r="B93" s="4" t="s">
         <v>602</v>
       </c>
-      <c r="C84" s="4" t="s">
+      <c r="C93" s="4" t="s">
         <v>605</v>
       </c>
-      <c r="N84" s="4" t="s">
+      <c r="N93" s="4" t="s">
         <v>776</v>
       </c>
-      <c r="O84" s="5"/>
-    </row>
-    <row r="85" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B85" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C85" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="D85" s="8" t="s">
-        <v>501</v>
-      </c>
-      <c r="E85" s="8" t="s">
-        <v>470</v>
-      </c>
-      <c r="F85" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="G85" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="H85" s="8" t="s">
-        <v>407</v>
-      </c>
-      <c r="K85" s="10" t="s">
-        <v>562</v>
-      </c>
-      <c r="L85" s="10" t="s">
-        <v>652</v>
-      </c>
-      <c r="M85" s="10"/>
-      <c r="N85" s="10" t="s">
-        <v>439</v>
-      </c>
-      <c r="O85" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="P85" s="8" t="s">
-        <v>375</v>
-      </c>
-      <c r="Q85" s="8" t="s">
-        <v>217</v>
-      </c>
-      <c r="S85" s="7" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="86" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B86" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C86" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D86" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E86" s="8" t="s">
-        <v>471</v>
-      </c>
-      <c r="F86" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="G86" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="H86" s="8" t="s">
-        <v>408</v>
-      </c>
-      <c r="K86" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="L86" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="M86" s="10"/>
-      <c r="N86" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="O86" s="8" t="s">
-        <v>531</v>
-      </c>
-      <c r="P86" s="8" t="s">
-        <v>376</v>
-      </c>
-      <c r="Q86" s="8" t="s">
-        <v>218</v>
-      </c>
-      <c r="S86" s="7" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="87" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B87" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C87" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="D87" s="8" t="s">
-        <v>502</v>
-      </c>
-      <c r="E87" s="8" t="s">
-        <v>472</v>
-      </c>
-      <c r="F87" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="G87" s="8" t="s">
-        <v>187</v>
-      </c>
-      <c r="H87" s="8" t="s">
-        <v>409</v>
-      </c>
-      <c r="K87" s="10" t="s">
-        <v>563</v>
-      </c>
-      <c r="L87" s="10" t="s">
-        <v>653</v>
-      </c>
-      <c r="M87" s="10"/>
-      <c r="N87" s="10" t="s">
-        <v>440</v>
-      </c>
-      <c r="O87" s="8" t="s">
-        <v>532</v>
-      </c>
-      <c r="P87" s="8" t="s">
-        <v>377</v>
-      </c>
-      <c r="Q87" s="8" t="s">
-        <v>219</v>
-      </c>
-      <c r="S87" s="7" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="88" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B88" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C88" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="D88" s="8" t="s">
-        <v>503</v>
-      </c>
-      <c r="E88" s="8" t="s">
-        <v>473</v>
-      </c>
-      <c r="F88" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="G88" s="8" t="s">
-        <v>188</v>
-      </c>
-      <c r="H88" s="8" t="s">
-        <v>410</v>
-      </c>
-      <c r="K88" s="10" t="s">
-        <v>564</v>
-      </c>
-      <c r="L88" s="10" t="s">
-        <v>654</v>
-      </c>
-      <c r="M88" s="10"/>
-      <c r="N88" s="10" t="s">
-        <v>441</v>
-      </c>
-      <c r="O88" s="8" t="s">
-        <v>533</v>
-      </c>
-      <c r="P88" s="8" t="s">
-        <v>378</v>
-      </c>
-      <c r="Q88" s="8" t="s">
-        <v>220</v>
-      </c>
-      <c r="S88" s="7" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="89" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B89" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C89" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="D89" s="8" t="s">
-        <v>504</v>
-      </c>
-      <c r="E89" s="8" t="s">
-        <v>474</v>
-      </c>
-      <c r="F89" s="8" t="s">
-        <v>159</v>
-      </c>
-      <c r="G89" s="8" t="s">
-        <v>189</v>
-      </c>
-      <c r="H89" s="8" t="s">
-        <v>411</v>
-      </c>
-      <c r="K89" s="10" t="s">
-        <v>565</v>
-      </c>
-      <c r="L89" s="10" t="s">
-        <v>655</v>
-      </c>
-      <c r="M89" s="10"/>
-      <c r="N89" s="10" t="s">
-        <v>442</v>
-      </c>
-      <c r="O89" s="8" t="s">
-        <v>534</v>
-      </c>
-      <c r="P89" s="8" t="s">
-        <v>379</v>
-      </c>
-      <c r="Q89" s="8" t="s">
-        <v>221</v>
-      </c>
-      <c r="S89" s="7" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="90" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="B90" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="C90" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="D90" s="8" t="s">
-        <v>505</v>
-      </c>
-      <c r="E90" s="8" t="s">
-        <v>475</v>
-      </c>
-      <c r="F90" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="G90" s="8" t="s">
-        <v>190</v>
-      </c>
-      <c r="H90" s="8" t="s">
-        <v>412</v>
-      </c>
-      <c r="K90" s="10" t="s">
-        <v>566</v>
-      </c>
-      <c r="L90" s="10" t="s">
-        <v>656</v>
-      </c>
-      <c r="M90" s="10"/>
-      <c r="N90" s="10" t="s">
-        <v>443</v>
-      </c>
-      <c r="O90" s="8" t="s">
-        <v>535</v>
-      </c>
-      <c r="P90" s="8" t="s">
-        <v>380</v>
-      </c>
-      <c r="Q90" s="8" t="s">
-        <v>222</v>
-      </c>
-      <c r="S90" s="7" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="91" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B91" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C91" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="D91" s="8" t="s">
-        <v>506</v>
-      </c>
-      <c r="E91" s="8" t="s">
-        <v>476</v>
-      </c>
-      <c r="F91" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="G91" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="H91" s="8" t="s">
-        <v>413</v>
-      </c>
-      <c r="K91" s="10" t="s">
-        <v>567</v>
-      </c>
-      <c r="L91" s="10" t="s">
-        <v>657</v>
-      </c>
-      <c r="M91" s="10"/>
-      <c r="N91" s="10" t="s">
-        <v>444</v>
-      </c>
-      <c r="O91" s="8" t="s">
-        <v>536</v>
-      </c>
-      <c r="P91" s="8" t="s">
-        <v>381</v>
-      </c>
-      <c r="Q91" s="8" t="s">
-        <v>223</v>
-      </c>
-      <c r="S91" s="7" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="92" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B92" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C92" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="D92" s="8" t="s">
-        <v>507</v>
-      </c>
-      <c r="E92" s="8" t="s">
-        <v>477</v>
-      </c>
-      <c r="F92" s="8" t="s">
-        <v>162</v>
-      </c>
-      <c r="G92" s="8" t="s">
-        <v>192</v>
-      </c>
-      <c r="H92" s="8" t="s">
-        <v>414</v>
-      </c>
-      <c r="K92" s="10" t="s">
-        <v>568</v>
-      </c>
-      <c r="L92" s="10" t="s">
-        <v>658</v>
-      </c>
-      <c r="M92" s="10"/>
-      <c r="N92" s="10" t="s">
-        <v>445</v>
-      </c>
-      <c r="O92" s="8" t="s">
-        <v>537</v>
-      </c>
-      <c r="P92" s="8" t="s">
-        <v>382</v>
-      </c>
-      <c r="Q92" s="8" t="s">
-        <v>224</v>
-      </c>
-      <c r="S92" s="7" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="93" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B93" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C93" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="D93" s="8" t="s">
-        <v>508</v>
-      </c>
-      <c r="E93" s="8" t="s">
-        <v>478</v>
-      </c>
-      <c r="F93" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="G93" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="H93" s="8" t="s">
-        <v>415</v>
-      </c>
-      <c r="K93" s="10" t="s">
-        <v>569</v>
-      </c>
-      <c r="L93" s="10" t="s">
-        <v>659</v>
-      </c>
-      <c r="M93" s="10"/>
-      <c r="N93" s="10" t="s">
-        <v>446</v>
-      </c>
-      <c r="O93" s="8" t="s">
-        <v>538</v>
-      </c>
-      <c r="P93" s="8" t="s">
-        <v>383</v>
-      </c>
-      <c r="Q93" s="8" t="s">
-        <v>225</v>
-      </c>
-      <c r="S93" s="7" t="s">
-        <v>351</v>
-      </c>
+      <c r="O93" s="5"/>
     </row>
     <row r="94" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="6" t="s">
-        <v>11</v>
+        <v>59</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="C94" s="8" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="D94" s="8" t="s">
-        <v>509</v>
+        <v>501</v>
       </c>
       <c r="E94" s="8" t="s">
-        <v>479</v>
+        <v>470</v>
       </c>
       <c r="F94" s="8" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="G94" s="8" t="s">
-        <v>194</v>
+        <v>60</v>
       </c>
       <c r="H94" s="8" t="s">
-        <v>416</v>
+        <v>407</v>
       </c>
       <c r="K94" s="10" t="s">
-        <v>570</v>
+        <v>562</v>
       </c>
       <c r="L94" s="10" t="s">
-        <v>660</v>
+        <v>652</v>
       </c>
       <c r="M94" s="10"/>
       <c r="N94" s="10" t="s">
-        <v>447</v>
+        <v>439</v>
       </c>
       <c r="O94" s="8" t="s">
-        <v>539</v>
+        <v>155</v>
       </c>
       <c r="P94" s="8" t="s">
-        <v>384</v>
+        <v>375</v>
       </c>
       <c r="Q94" s="8" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="S94" s="7" t="s">
-        <v>352</v>
+        <v>343</v>
       </c>
     </row>
     <row r="95" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="6" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="C95" s="8" t="s">
-        <v>130</v>
+        <v>7</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>505</v>
+        <v>7</v>
       </c>
       <c r="E95" s="8" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="F95" s="8" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="G95" s="8" t="s">
-        <v>190</v>
+        <v>7</v>
       </c>
       <c r="H95" s="8" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="K95" s="10" t="s">
-        <v>571</v>
+        <v>7</v>
       </c>
       <c r="L95" s="10" t="s">
-        <v>656</v>
+        <v>7</v>
       </c>
       <c r="M95" s="10"/>
       <c r="N95" s="10" t="s">
-        <v>443</v>
+        <v>7</v>
       </c>
       <c r="O95" s="8" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="P95" s="8" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="Q95" s="8" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="S95" s="7" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="96" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="6" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C96" s="8" t="s">
-        <v>271</v>
+        <v>127</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>510</v>
+        <v>502</v>
       </c>
       <c r="E96" s="8" t="s">
-        <v>480</v>
+        <v>472</v>
       </c>
       <c r="F96" s="8" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="G96" s="8" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="H96" s="8" t="s">
-        <v>417</v>
+        <v>409</v>
       </c>
       <c r="K96" s="10" t="s">
-        <v>572</v>
+        <v>563</v>
       </c>
       <c r="L96" s="10" t="s">
-        <v>661</v>
+        <v>653</v>
       </c>
       <c r="M96" s="10"/>
       <c r="N96" s="10" t="s">
-        <v>448</v>
+        <v>440</v>
       </c>
       <c r="O96" s="8" t="s">
-        <v>540</v>
+        <v>532</v>
       </c>
       <c r="P96" s="8" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="Q96" s="8" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="S96" s="7" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
     </row>
     <row r="97" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="6" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C97" s="8" t="s">
-        <v>270</v>
+        <v>128</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>511</v>
+        <v>503</v>
       </c>
       <c r="E97" s="8" t="s">
-        <v>481</v>
+        <v>473</v>
       </c>
       <c r="F97" s="8" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="G97" s="8" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="H97" s="8" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
       <c r="K97" s="10" t="s">
-        <v>573</v>
+        <v>564</v>
       </c>
       <c r="L97" s="10" t="s">
-        <v>662</v>
+        <v>654</v>
       </c>
       <c r="M97" s="10"/>
       <c r="N97" s="10" t="s">
-        <v>449</v>
+        <v>441</v>
       </c>
       <c r="O97" s="8" t="s">
-        <v>541</v>
+        <v>533</v>
       </c>
       <c r="P97" s="8" t="s">
-        <v>386</v>
+        <v>378</v>
       </c>
       <c r="Q97" s="8" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="S97" s="7" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
     </row>
     <row r="98" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="6" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C98" s="8" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="D98" s="8" t="s">
-        <v>512</v>
+        <v>504</v>
       </c>
       <c r="E98" s="8" t="s">
-        <v>482</v>
+        <v>474</v>
       </c>
       <c r="F98" s="8" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="G98" s="8" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="H98" s="8" t="s">
-        <v>419</v>
+        <v>411</v>
       </c>
       <c r="K98" s="10" t="s">
-        <v>574</v>
+        <v>565</v>
       </c>
       <c r="L98" s="10" t="s">
-        <v>663</v>
+        <v>655</v>
       </c>
       <c r="M98" s="10"/>
       <c r="N98" s="10" t="s">
-        <v>450</v>
+        <v>442</v>
       </c>
       <c r="O98" s="8" t="s">
-        <v>542</v>
+        <v>534</v>
       </c>
       <c r="P98" s="8" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="Q98" s="8" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="S98" s="7" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
     </row>
     <row r="99" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="6" t="s">
-        <v>16</v>
+        <v>62</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="C99" s="8" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="D99" s="8" t="s">
-        <v>513</v>
+        <v>505</v>
       </c>
       <c r="E99" s="8" t="s">
-        <v>483</v>
+        <v>475</v>
       </c>
       <c r="F99" s="8" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="G99" s="8" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="H99" s="8" t="s">
-        <v>420</v>
+        <v>412</v>
       </c>
       <c r="K99" s="10" t="s">
-        <v>575</v>
+        <v>566</v>
       </c>
       <c r="L99" s="10" t="s">
-        <v>664</v>
+        <v>656</v>
       </c>
       <c r="M99" s="10"/>
       <c r="N99" s="10" t="s">
-        <v>451</v>
+        <v>443</v>
       </c>
       <c r="O99" s="8" t="s">
-        <v>543</v>
+        <v>535</v>
       </c>
       <c r="P99" s="8" t="s">
-        <v>388</v>
+        <v>380</v>
       </c>
       <c r="Q99" s="8" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="S99" s="7" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
     </row>
     <row r="100" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="6" t="s">
-        <v>64</v>
+        <v>8</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="C100" s="8" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="D100" s="8" t="s">
-        <v>514</v>
+        <v>506</v>
       </c>
       <c r="E100" s="8" t="s">
-        <v>484</v>
+        <v>476</v>
       </c>
       <c r="F100" s="8" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="G100" s="8" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="H100" s="8" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
       <c r="K100" s="10" t="s">
-        <v>576</v>
+        <v>567</v>
       </c>
       <c r="L100" s="10" t="s">
-        <v>665</v>
+        <v>657</v>
       </c>
       <c r="M100" s="10"/>
       <c r="N100" s="10" t="s">
-        <v>452</v>
+        <v>444</v>
       </c>
       <c r="O100" s="8" t="s">
-        <v>544</v>
+        <v>536</v>
       </c>
       <c r="P100" s="8" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
       <c r="Q100" s="8" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="S100" s="7" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
     </row>
     <row r="101" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="6" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C101" s="8" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="D101" s="8" t="s">
-        <v>515</v>
+        <v>507</v>
       </c>
       <c r="E101" s="8" t="s">
-        <v>485</v>
+        <v>477</v>
       </c>
       <c r="F101" s="8" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="G101" s="8" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="H101" s="8" t="s">
-        <v>422</v>
+        <v>414</v>
       </c>
       <c r="K101" s="10" t="s">
-        <v>577</v>
+        <v>568</v>
       </c>
       <c r="L101" s="10" t="s">
-        <v>666</v>
+        <v>658</v>
       </c>
       <c r="M101" s="10"/>
       <c r="N101" s="10" t="s">
-        <v>453</v>
+        <v>445</v>
       </c>
       <c r="O101" s="8" t="s">
-        <v>545</v>
+        <v>537</v>
       </c>
       <c r="P101" s="8" t="s">
-        <v>390</v>
+        <v>382</v>
       </c>
       <c r="Q101" s="8" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="S101" s="7" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
     </row>
     <row r="102" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="6" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="C102" s="8" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="D102" s="8" t="s">
-        <v>516</v>
+        <v>508</v>
       </c>
       <c r="E102" s="8" t="s">
-        <v>486</v>
+        <v>478</v>
       </c>
       <c r="F102" s="8" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="G102" s="8" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="H102" s="8" t="s">
-        <v>423</v>
+        <v>415</v>
       </c>
       <c r="K102" s="10" t="s">
-        <v>578</v>
+        <v>569</v>
       </c>
       <c r="L102" s="10" t="s">
-        <v>667</v>
+        <v>659</v>
       </c>
       <c r="M102" s="10"/>
       <c r="N102" s="10" t="s">
-        <v>454</v>
+        <v>446</v>
       </c>
       <c r="O102" s="8" t="s">
-        <v>546</v>
+        <v>538</v>
       </c>
       <c r="P102" s="8" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
       <c r="Q102" s="8" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="S102" s="7" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
     </row>
     <row r="103" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="6" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="C103" s="8" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="D103" s="8" t="s">
-        <v>517</v>
+        <v>509</v>
       </c>
       <c r="E103" s="8" t="s">
-        <v>487</v>
+        <v>479</v>
       </c>
       <c r="F103" s="8" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="G103" s="8" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="H103" s="8" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
       <c r="K103" s="10" t="s">
-        <v>579</v>
+        <v>570</v>
       </c>
       <c r="L103" s="10" t="s">
-        <v>668</v>
+        <v>660</v>
       </c>
       <c r="M103" s="10"/>
       <c r="N103" s="10" t="s">
-        <v>455</v>
+        <v>447</v>
       </c>
       <c r="O103" s="8" t="s">
-        <v>547</v>
+        <v>539</v>
       </c>
       <c r="P103" s="8" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
       <c r="Q103" s="8" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="S103" s="7" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
     </row>
     <row r="104" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="6" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B104" s="7" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C104" s="8" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="D104" s="8" t="s">
-        <v>518</v>
+        <v>505</v>
       </c>
       <c r="E104" s="8" t="s">
-        <v>488</v>
+        <v>475</v>
       </c>
       <c r="F104" s="8" t="s">
-        <v>173</v>
+        <v>160</v>
       </c>
       <c r="G104" s="8" t="s">
-        <v>203</v>
+        <v>190</v>
       </c>
       <c r="H104" s="8" t="s">
-        <v>425</v>
+        <v>412</v>
       </c>
       <c r="K104" s="10" t="s">
-        <v>580</v>
+        <v>571</v>
       </c>
       <c r="L104" s="10" t="s">
-        <v>669</v>
+        <v>656</v>
       </c>
       <c r="M104" s="10"/>
       <c r="N104" s="10" t="s">
-        <v>456</v>
+        <v>443</v>
       </c>
       <c r="O104" s="8" t="s">
-        <v>548</v>
+        <v>535</v>
       </c>
       <c r="P104" s="8" t="s">
-        <v>393</v>
+        <v>380</v>
       </c>
       <c r="Q104" s="8" t="s">
-        <v>235</v>
+        <v>222</v>
       </c>
       <c r="S104" s="7" t="s">
-        <v>361</v>
+        <v>348</v>
       </c>
     </row>
     <row r="105" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="6" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B105" s="7" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C105" s="8" t="s">
-        <v>142</v>
+        <v>271</v>
       </c>
       <c r="D105" s="8" t="s">
-        <v>519</v>
+        <v>510</v>
       </c>
       <c r="E105" s="8" t="s">
-        <v>489</v>
+        <v>480</v>
       </c>
       <c r="F105" s="8" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="G105" s="8" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="H105" s="8" t="s">
-        <v>426</v>
+        <v>417</v>
       </c>
       <c r="K105" s="10" t="s">
-        <v>581</v>
+        <v>572</v>
       </c>
       <c r="L105" s="10" t="s">
-        <v>670</v>
+        <v>661</v>
       </c>
       <c r="M105" s="10"/>
       <c r="N105" s="10" t="s">
-        <v>457</v>
+        <v>448</v>
       </c>
       <c r="O105" s="8" t="s">
-        <v>549</v>
+        <v>540</v>
       </c>
       <c r="P105" s="8" t="s">
-        <v>394</v>
+        <v>385</v>
       </c>
       <c r="Q105" s="8" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="S105" s="7" t="s">
-        <v>362</v>
+        <v>353</v>
       </c>
     </row>
     <row r="106" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="6" t="s">
-        <v>65</v>
+        <v>14</v>
       </c>
       <c r="B106" s="7" t="s">
-        <v>275</v>
+        <v>37</v>
       </c>
       <c r="C106" s="8" t="s">
-        <v>143</v>
+        <v>270</v>
       </c>
       <c r="D106" s="8" t="s">
-        <v>458</v>
+        <v>511</v>
       </c>
       <c r="E106" s="8" t="s">
-        <v>490</v>
+        <v>481</v>
       </c>
       <c r="F106" s="8" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="G106" s="8" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="H106" s="8" t="s">
-        <v>427</v>
+        <v>418</v>
       </c>
       <c r="K106" s="10" t="s">
-        <v>582</v>
+        <v>573</v>
       </c>
       <c r="L106" s="10" t="s">
-        <v>671</v>
+        <v>662</v>
       </c>
       <c r="M106" s="10"/>
       <c r="N106" s="10" t="s">
-        <v>458</v>
+        <v>449</v>
       </c>
       <c r="O106" s="8" t="s">
-        <v>550</v>
+        <v>541</v>
       </c>
       <c r="P106" s="8" t="s">
-        <v>395</v>
+        <v>386</v>
       </c>
       <c r="Q106" s="8" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="S106" s="7" t="s">
-        <v>363</v>
+        <v>354</v>
       </c>
     </row>
     <row r="107" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="6" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="C107" s="8" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="D107" s="8" t="s">
-        <v>520</v>
+        <v>512</v>
       </c>
       <c r="E107" s="8" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="F107" s="8" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="G107" s="8" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="H107" s="8" t="s">
-        <v>428</v>
+        <v>419</v>
       </c>
       <c r="K107" s="10" t="s">
-        <v>583</v>
+        <v>574</v>
       </c>
       <c r="L107" s="10" t="s">
-        <v>672</v>
+        <v>663</v>
       </c>
       <c r="M107" s="10"/>
       <c r="N107" s="10" t="s">
-        <v>459</v>
+        <v>450</v>
       </c>
       <c r="O107" s="8" t="s">
-        <v>551</v>
+        <v>542</v>
       </c>
       <c r="P107" s="8" t="s">
-        <v>396</v>
+        <v>387</v>
       </c>
       <c r="Q107" s="8" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="S107" s="7" t="s">
-        <v>364</v>
+        <v>355</v>
       </c>
     </row>
     <row r="108" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="6" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="C108" s="8" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="D108" s="8" t="s">
-        <v>521</v>
+        <v>513</v>
       </c>
       <c r="E108" s="8" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
       <c r="F108" s="8" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="G108" s="8" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="H108" s="8" t="s">
-        <v>429</v>
+        <v>420</v>
       </c>
       <c r="K108" s="10" t="s">
-        <v>584</v>
+        <v>575</v>
       </c>
       <c r="L108" s="10" t="s">
-        <v>673</v>
+        <v>664</v>
       </c>
       <c r="M108" s="10"/>
       <c r="N108" s="10" t="s">
-        <v>460</v>
+        <v>451</v>
       </c>
       <c r="O108" s="8" t="s">
-        <v>552</v>
+        <v>543</v>
       </c>
       <c r="P108" s="8" t="s">
-        <v>397</v>
+        <v>388</v>
       </c>
       <c r="Q108" s="8" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="S108" s="7" t="s">
-        <v>365</v>
+        <v>356</v>
       </c>
     </row>
     <row r="109" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="6" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="C109" s="8" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="D109" s="8" t="s">
-        <v>522</v>
+        <v>514</v>
       </c>
       <c r="E109" s="8" t="s">
-        <v>493</v>
+        <v>484</v>
       </c>
       <c r="F109" s="8" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="G109" s="8" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="H109" s="8" t="s">
-        <v>430</v>
+        <v>421</v>
       </c>
       <c r="K109" s="10" t="s">
-        <v>585</v>
+        <v>576</v>
       </c>
       <c r="L109" s="10" t="s">
-        <v>674</v>
+        <v>665</v>
       </c>
       <c r="M109" s="10"/>
       <c r="N109" s="10" t="s">
-        <v>461</v>
+        <v>452</v>
       </c>
       <c r="O109" s="8" t="s">
-        <v>553</v>
+        <v>544</v>
       </c>
       <c r="P109" s="8" t="s">
-        <v>398</v>
+        <v>389</v>
       </c>
       <c r="Q109" s="8" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="S109" s="7" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
     </row>
     <row r="110" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="6" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B110" s="7" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C110" s="8" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="D110" s="8" t="s">
-        <v>523</v>
+        <v>515</v>
       </c>
       <c r="E110" s="8" t="s">
-        <v>493</v>
+        <v>485</v>
       </c>
       <c r="F110" s="8" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="G110" s="8" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="H110" s="8" t="s">
-        <v>431</v>
+        <v>422</v>
       </c>
       <c r="K110" s="10" t="s">
-        <v>586</v>
+        <v>577</v>
       </c>
       <c r="L110" s="10" t="s">
-        <v>675</v>
+        <v>666</v>
       </c>
       <c r="M110" s="10"/>
       <c r="N110" s="10" t="s">
-        <v>462</v>
+        <v>453</v>
       </c>
       <c r="O110" s="8" t="s">
-        <v>554</v>
+        <v>545</v>
       </c>
       <c r="P110" s="8" t="s">
-        <v>399</v>
+        <v>390</v>
       </c>
       <c r="Q110" s="8" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="S110" s="7" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
     </row>
     <row r="111" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="6" t="s">
-        <v>66</v>
+        <v>18</v>
       </c>
       <c r="B111" s="7" t="s">
-        <v>67</v>
+        <v>40</v>
       </c>
       <c r="C111" s="8" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="D111" s="8" t="s">
-        <v>524</v>
+        <v>516</v>
       </c>
       <c r="E111" s="8" t="s">
-        <v>494</v>
+        <v>486</v>
       </c>
       <c r="F111" s="8" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="G111" s="8" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="H111" s="8" t="s">
-        <v>432</v>
+        <v>423</v>
       </c>
       <c r="K111" s="10" t="s">
-        <v>587</v>
+        <v>578</v>
       </c>
       <c r="L111" s="10" t="s">
-        <v>676</v>
+        <v>667</v>
       </c>
       <c r="M111" s="10"/>
       <c r="N111" s="10" t="s">
-        <v>463</v>
+        <v>454</v>
       </c>
       <c r="O111" s="8" t="s">
-        <v>555</v>
+        <v>546</v>
       </c>
       <c r="P111" s="8" t="s">
-        <v>400</v>
+        <v>391</v>
       </c>
       <c r="Q111" s="8" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="S111" s="7" t="s">
-        <v>368</v>
+        <v>359</v>
       </c>
     </row>
     <row r="112" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A112" s="6" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B112" s="7" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="C112" s="8" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="D112" s="8" t="s">
-        <v>525</v>
+        <v>517</v>
       </c>
       <c r="E112" s="8" t="s">
-        <v>495</v>
+        <v>487</v>
       </c>
       <c r="F112" s="8" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="G112" s="8" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="H112" s="8" t="s">
-        <v>433</v>
+        <v>424</v>
       </c>
       <c r="K112" s="10" t="s">
-        <v>588</v>
+        <v>579</v>
       </c>
       <c r="L112" s="10" t="s">
-        <v>677</v>
+        <v>668</v>
       </c>
       <c r="M112" s="10"/>
       <c r="N112" s="10" t="s">
-        <v>464</v>
+        <v>455</v>
       </c>
       <c r="O112" s="8" t="s">
-        <v>556</v>
+        <v>547</v>
       </c>
       <c r="P112" s="8" t="s">
-        <v>401</v>
+        <v>392</v>
       </c>
       <c r="Q112" s="8" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="S112" s="7" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
     </row>
     <row r="113" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A113" s="6" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B113" s="7" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="C113" s="8" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="D113" s="8" t="s">
-        <v>526</v>
+        <v>518</v>
       </c>
       <c r="E113" s="8" t="s">
-        <v>496</v>
+        <v>488</v>
       </c>
       <c r="F113" s="8" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="G113" s="8" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="H113" s="8" t="s">
-        <v>434</v>
+        <v>425</v>
       </c>
       <c r="K113" s="10" t="s">
-        <v>589</v>
+        <v>580</v>
       </c>
       <c r="L113" s="10" t="s">
-        <v>678</v>
+        <v>669</v>
       </c>
       <c r="M113" s="10"/>
       <c r="N113" s="10" t="s">
-        <v>465</v>
+        <v>456</v>
       </c>
       <c r="O113" s="8" t="s">
-        <v>557</v>
+        <v>548</v>
       </c>
       <c r="P113" s="8" t="s">
-        <v>402</v>
+        <v>393</v>
       </c>
       <c r="Q113" s="8" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="S113" s="7" t="s">
-        <v>370</v>
+        <v>361</v>
       </c>
     </row>
     <row r="114" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A114" s="6" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B114" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C114" s="8" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="D114" s="8" t="s">
-        <v>527</v>
+        <v>519</v>
       </c>
       <c r="E114" s="8" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
       <c r="F114" s="8" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="G114" s="8" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="H114" s="8" t="s">
-        <v>435</v>
+        <v>426</v>
       </c>
       <c r="K114" s="10" t="s">
-        <v>590</v>
+        <v>581</v>
       </c>
       <c r="L114" s="10" t="s">
-        <v>679</v>
+        <v>670</v>
       </c>
       <c r="M114" s="10"/>
       <c r="N114" s="10" t="s">
-        <v>466</v>
+        <v>457</v>
       </c>
       <c r="O114" s="8" t="s">
-        <v>558</v>
+        <v>549</v>
       </c>
       <c r="P114" s="8" t="s">
-        <v>403</v>
+        <v>394</v>
       </c>
       <c r="Q114" s="8" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="S114" s="7" t="s">
-        <v>371</v>
+        <v>362</v>
       </c>
     </row>
     <row r="115" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A115" s="6" t="s">
-        <v>29</v>
+        <v>65</v>
       </c>
       <c r="B115" s="7" t="s">
-        <v>45</v>
+        <v>275</v>
       </c>
       <c r="C115" s="8" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="D115" s="8" t="s">
-        <v>528</v>
+        <v>458</v>
       </c>
       <c r="E115" s="8" t="s">
-        <v>498</v>
+        <v>490</v>
       </c>
       <c r="F115" s="8" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="G115" s="8" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="H115" s="8" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
       <c r="K115" s="10" t="s">
-        <v>591</v>
+        <v>582</v>
       </c>
       <c r="L115" s="10" t="s">
-        <v>680</v>
+        <v>671</v>
       </c>
       <c r="M115" s="10"/>
       <c r="N115" s="10" t="s">
-        <v>467</v>
+        <v>458</v>
       </c>
       <c r="O115" s="8" t="s">
-        <v>559</v>
+        <v>550</v>
       </c>
       <c r="P115" s="8" t="s">
-        <v>404</v>
+        <v>395</v>
       </c>
       <c r="Q115" s="8" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="S115" s="7" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
     </row>
     <row r="116" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A116" s="6" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B116" s="7" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C116" s="8" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="D116" s="8" t="s">
-        <v>529</v>
+        <v>520</v>
       </c>
       <c r="E116" s="8" t="s">
-        <v>499</v>
+        <v>491</v>
       </c>
       <c r="F116" s="8" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="G116" s="8" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="H116" s="8" t="s">
-        <v>437</v>
+        <v>428</v>
       </c>
       <c r="K116" s="10" t="s">
-        <v>592</v>
+        <v>583</v>
       </c>
       <c r="L116" s="10" t="s">
-        <v>681</v>
+        <v>672</v>
       </c>
       <c r="M116" s="10"/>
       <c r="N116" s="10" t="s">
-        <v>468</v>
+        <v>459</v>
       </c>
       <c r="O116" s="8" t="s">
-        <v>560</v>
+        <v>551</v>
       </c>
       <c r="P116" s="8" t="s">
-        <v>405</v>
+        <v>396</v>
       </c>
       <c r="Q116" s="8" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="S116" s="7" t="s">
-        <v>373</v>
+        <v>364</v>
       </c>
     </row>
     <row r="117" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A117" s="6" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B117" s="7" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C117" s="8" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="D117" s="8" t="s">
-        <v>530</v>
+        <v>521</v>
       </c>
       <c r="E117" s="8" t="s">
-        <v>500</v>
+        <v>492</v>
       </c>
       <c r="F117" s="8" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="G117" s="8" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="H117" s="8" t="s">
-        <v>438</v>
+        <v>429</v>
       </c>
       <c r="K117" s="10" t="s">
-        <v>593</v>
+        <v>584</v>
       </c>
       <c r="L117" s="10" t="s">
-        <v>682</v>
+        <v>673</v>
       </c>
       <c r="M117" s="10"/>
       <c r="N117" s="10" t="s">
+        <v>460</v>
+      </c>
+      <c r="O117" s="8" t="s">
+        <v>552</v>
+      </c>
+      <c r="P117" s="8" t="s">
+        <v>397</v>
+      </c>
+      <c r="Q117" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="S117" s="7" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="118" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B118" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C118" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="D118" s="8" t="s">
+        <v>522</v>
+      </c>
+      <c r="E118" s="8" t="s">
+        <v>493</v>
+      </c>
+      <c r="F118" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="G118" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="H118" s="8" t="s">
+        <v>430</v>
+      </c>
+      <c r="K118" s="10" t="s">
+        <v>585</v>
+      </c>
+      <c r="L118" s="10" t="s">
+        <v>674</v>
+      </c>
+      <c r="M118" s="10"/>
+      <c r="N118" s="10" t="s">
+        <v>461</v>
+      </c>
+      <c r="O118" s="8" t="s">
+        <v>553</v>
+      </c>
+      <c r="P118" s="8" t="s">
+        <v>398</v>
+      </c>
+      <c r="Q118" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="S118" s="7" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="119" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B119" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C119" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="D119" s="8" t="s">
+        <v>523</v>
+      </c>
+      <c r="E119" s="8" t="s">
+        <v>493</v>
+      </c>
+      <c r="F119" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="G119" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="H119" s="8" t="s">
+        <v>431</v>
+      </c>
+      <c r="K119" s="10" t="s">
+        <v>586</v>
+      </c>
+      <c r="L119" s="10" t="s">
+        <v>675</v>
+      </c>
+      <c r="M119" s="10"/>
+      <c r="N119" s="10" t="s">
+        <v>462</v>
+      </c>
+      <c r="O119" s="8" t="s">
+        <v>554</v>
+      </c>
+      <c r="P119" s="8" t="s">
+        <v>399</v>
+      </c>
+      <c r="Q119" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="S119" s="7" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="120" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B120" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C120" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="D120" s="8" t="s">
+        <v>524</v>
+      </c>
+      <c r="E120" s="8" t="s">
+        <v>494</v>
+      </c>
+      <c r="F120" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="G120" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="H120" s="8" t="s">
+        <v>432</v>
+      </c>
+      <c r="K120" s="10" t="s">
+        <v>587</v>
+      </c>
+      <c r="L120" s="10" t="s">
+        <v>676</v>
+      </c>
+      <c r="M120" s="10"/>
+      <c r="N120" s="10" t="s">
+        <v>463</v>
+      </c>
+      <c r="O120" s="8" t="s">
+        <v>555</v>
+      </c>
+      <c r="P120" s="8" t="s">
+        <v>400</v>
+      </c>
+      <c r="Q120" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="S120" s="7" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="121" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B121" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C121" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="D121" s="8" t="s">
+        <v>525</v>
+      </c>
+      <c r="E121" s="8" t="s">
+        <v>495</v>
+      </c>
+      <c r="F121" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="G121" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="H121" s="8" t="s">
+        <v>433</v>
+      </c>
+      <c r="K121" s="10" t="s">
+        <v>588</v>
+      </c>
+      <c r="L121" s="10" t="s">
+        <v>677</v>
+      </c>
+      <c r="M121" s="10"/>
+      <c r="N121" s="10" t="s">
+        <v>464</v>
+      </c>
+      <c r="O121" s="8" t="s">
+        <v>556</v>
+      </c>
+      <c r="P121" s="8" t="s">
+        <v>401</v>
+      </c>
+      <c r="Q121" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="S121" s="7" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="122" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B122" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C122" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="D122" s="8" t="s">
+        <v>526</v>
+      </c>
+      <c r="E122" s="8" t="s">
+        <v>496</v>
+      </c>
+      <c r="F122" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="G122" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="H122" s="8" t="s">
+        <v>434</v>
+      </c>
+      <c r="K122" s="10" t="s">
+        <v>589</v>
+      </c>
+      <c r="L122" s="10" t="s">
+        <v>678</v>
+      </c>
+      <c r="M122" s="10"/>
+      <c r="N122" s="10" t="s">
+        <v>465</v>
+      </c>
+      <c r="O122" s="8" t="s">
+        <v>557</v>
+      </c>
+      <c r="P122" s="8" t="s">
+        <v>402</v>
+      </c>
+      <c r="Q122" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="S122" s="7" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="123" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B123" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C123" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="D123" s="8" t="s">
+        <v>527</v>
+      </c>
+      <c r="E123" s="8" t="s">
+        <v>497</v>
+      </c>
+      <c r="F123" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="G123" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="H123" s="8" t="s">
+        <v>435</v>
+      </c>
+      <c r="K123" s="10" t="s">
+        <v>590</v>
+      </c>
+      <c r="L123" s="10" t="s">
+        <v>679</v>
+      </c>
+      <c r="M123" s="10"/>
+      <c r="N123" s="10" t="s">
+        <v>466</v>
+      </c>
+      <c r="O123" s="8" t="s">
+        <v>558</v>
+      </c>
+      <c r="P123" s="8" t="s">
+        <v>403</v>
+      </c>
+      <c r="Q123" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="S123" s="7" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="124" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B124" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C124" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="D124" s="8" t="s">
+        <v>528</v>
+      </c>
+      <c r="E124" s="8" t="s">
+        <v>498</v>
+      </c>
+      <c r="F124" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="G124" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="H124" s="8" t="s">
+        <v>436</v>
+      </c>
+      <c r="K124" s="10" t="s">
+        <v>591</v>
+      </c>
+      <c r="L124" s="10" t="s">
+        <v>680</v>
+      </c>
+      <c r="M124" s="10"/>
+      <c r="N124" s="10" t="s">
+        <v>467</v>
+      </c>
+      <c r="O124" s="8" t="s">
+        <v>559</v>
+      </c>
+      <c r="P124" s="8" t="s">
+        <v>404</v>
+      </c>
+      <c r="Q124" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="S124" s="7" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="125" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B125" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C125" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="D125" s="8" t="s">
+        <v>529</v>
+      </c>
+      <c r="E125" s="8" t="s">
+        <v>499</v>
+      </c>
+      <c r="F125" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="G125" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="H125" s="8" t="s">
+        <v>437</v>
+      </c>
+      <c r="K125" s="10" t="s">
+        <v>592</v>
+      </c>
+      <c r="L125" s="10" t="s">
+        <v>681</v>
+      </c>
+      <c r="M125" s="10"/>
+      <c r="N125" s="10" t="s">
+        <v>468</v>
+      </c>
+      <c r="O125" s="8" t="s">
+        <v>560</v>
+      </c>
+      <c r="P125" s="8" t="s">
+        <v>405</v>
+      </c>
+      <c r="Q125" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="S125" s="7" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="126" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B126" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C126" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="D126" s="8" t="s">
+        <v>530</v>
+      </c>
+      <c r="E126" s="8" t="s">
+        <v>500</v>
+      </c>
+      <c r="F126" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="G126" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="H126" s="8" t="s">
+        <v>438</v>
+      </c>
+      <c r="K126" s="10" t="s">
+        <v>593</v>
+      </c>
+      <c r="L126" s="10" t="s">
+        <v>682</v>
+      </c>
+      <c r="M126" s="10"/>
+      <c r="N126" s="10" t="s">
         <v>469</v>
       </c>
-      <c r="O117" s="8" t="s">
+      <c r="O126" s="8" t="s">
         <v>561</v>
       </c>
-      <c r="P117" s="8" t="s">
+      <c r="P126" s="8" t="s">
         <v>406</v>
       </c>
-      <c r="Q117" s="8" t="s">
+      <c r="Q126" s="8" t="s">
         <v>248</v>
       </c>
-      <c r="S117" s="7" t="s">
+      <c r="S126" s="7" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="118" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A118" s="3" t="s">
+    <row r="127" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A127" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="B118" s="4" t="s">
+      <c r="B127" s="4" t="s">
         <v>273</v>
       </c>
-      <c r="C118" s="4" t="s">
+      <c r="C127" s="4" t="s">
         <v>274</v>
       </c>
-      <c r="N118" s="4" t="s">
+      <c r="N127" s="4" t="s">
         <v>777</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:U1"/>
+  <autoFilter ref="A1:U127"/>
   <sortState ref="D1:U1">
     <sortCondition ref="U1"/>
   </sortState>

</xml_diff>

<commit_message>
New localizations added due to SEO
</commit_message>
<xml_diff>
--- a/private/INDIVIDUAL_LOCALIZATIONS_UI_1.xlsx
+++ b/private/INDIVIDUAL_LOCALIZATIONS_UI_1.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24435" windowHeight="11880"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24435" windowHeight="11880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INTL" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="882" uniqueCount="840">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="898" uniqueCount="854">
   <si>
     <t>en_US</t>
   </si>
@@ -2547,12 +2547,54 @@
   </si>
   <si>
     <t>Aktuell gestreamtes Match</t>
+  </si>
+  <si>
+    <t>Builds {patch} | LoL VVV</t>
+  </si>
+  <si>
+    <t>{nickName} {position} builds {patch}  | LoL VVV</t>
+  </si>
+  <si>
+    <t>meta.head.title.builds</t>
+  </si>
+  <si>
+    <t>meta.head.description.builds</t>
+  </si>
+  <si>
+    <t>meta.head.title.pro.builds</t>
+  </si>
+  <si>
+    <t>meta.head.description.pro.builds</t>
+  </si>
+  <si>
+    <t>Find recent Builds and Guides from Pro gamers for patch {patch}, which will improve your gameplay.</t>
+  </si>
+  <si>
+    <t>Find Builds of {nickName} ({firstName} {lastName}) for patch {patch}. {nickName} plays on lane {position}.</t>
+  </si>
+  <si>
+    <t>{nickName} Builds</t>
+  </si>
+  <si>
+    <t>header.pro.builds</t>
+  </si>
+  <si>
+    <t>header.champion.builds</t>
+  </si>
+  <si>
+    <t>{championName} Builds</t>
+  </si>
+  <si>
+    <t>{championName} {position} builds {patch}  | LoL VVV</t>
+  </si>
+  <si>
+    <t>Find Builds of {championName} at {positions} lane for patch {patch}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3008,14 +3050,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U132"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:U140"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B110" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomRight" activeCell="A133" sqref="A133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6046,8 +6088,72 @@
         <v>777</v>
       </c>
     </row>
+    <row r="133" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A133" s="3" t="s">
+        <v>842</v>
+      </c>
+      <c r="B133" s="9" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="134" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A134" s="3" t="s">
+        <v>843</v>
+      </c>
+      <c r="B134" s="9" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="135" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A135" s="3" t="s">
+        <v>844</v>
+      </c>
+      <c r="B135" s="9" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="136" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A136" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="B136" s="9" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="137" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A137" s="3" t="s">
+        <v>844</v>
+      </c>
+      <c r="B137" s="9" t="s">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="138" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A138" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="B138" s="9" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="139" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A139" s="3" t="s">
+        <v>849</v>
+      </c>
+      <c r="B139" s="9" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="140" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A140" s="3" t="s">
+        <v>850</v>
+      </c>
+      <c r="B140" s="9" t="s">
+        <v>851</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:U132"/>
+  <autoFilter ref="A1:U132" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <sortState ref="D1:U1">
     <sortCondition ref="U1"/>
   </sortState>

</xml_diff>